<commit_message>
added privacy page, documentation, and fixed alerts bug
</commit_message>
<xml_diff>
--- a/content/dcf_model_blank.xlsx
+++ b/content/dcf_model_blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeung\Documents\Programming\cash-flow-v3\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE93882-9A39-4970-9715-B996DF714987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177A32F4-5ADC-444D-8B17-002768426C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7710" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="8" xr2:uid="{0646DCF6-9E5E-439A-8C31-869D606F0004}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="1000" activeTab="5" xr2:uid="{0646DCF6-9E5E-439A-8C31-869D606F0004}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="272" r:id="rId1"/>
@@ -979,9 +979,6 @@
     <t>W</t>
   </si>
   <si>
-    <t>Note: Please adjust corporate tax rates.</t>
-  </si>
-  <si>
     <t>Forecasts as of (date)</t>
   </si>
   <si>
@@ -1121,6 +1118,9 @@
   </si>
   <si>
     <t>VE9UQUxfUkVWLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgmQ0lRLjAuSVFfQ1VSUkVOVF9QT1JUX0xFQVNFUy4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIHUNJUS4wLklRX0NBU0hfRklOQU4uLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBlDSVEuMC5JUV9DT01NT04uLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBxDSVEuMC5JUV9MVF9JTlZFU1QuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBVDSVEuMC5JUV9BUi4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIK0NJUS4wLklRX09USEVSX05PTl9PUEVSX0VYUF9TVVBQTC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkI</t>
+  </si>
+  <si>
+    <t>Note: Please input corporate tax rates.</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="72" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C21" s="50"/>
       <c r="D21" s="108"/>
@@ -5453,13 +5453,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74EC6BE-E931-459B-9911-101FA66B3EAA}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5798,7 +5795,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B29" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C29" s="132"/>
       <c r="D29" s="10" t="e">
@@ -5826,7 +5823,7 @@
     <row r="30" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B30" s="30"/>
       <c r="C30" s="171" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D30" s="236" t="e">
         <f>D31/D27</f>
@@ -6910,8 +6907,8 @@
   </sheetPr>
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7636,7 +7633,7 @@
       <c r="M42" s="72"/>
       <c r="N42" s="72"/>
       <c r="O42" s="189" t="s">
-        <v>282</v>
+        <v>329</v>
       </c>
       <c r="P42" s="262"/>
       <c r="Q42" s="262"/>
@@ -8511,106 +8508,106 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" t="s">
         <v>296</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>297</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>298</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>299</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>300</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>301</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>302</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>303</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>304</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>305</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>306</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>307</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>308</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>309</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>310</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>311</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>312</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>313</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>314</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>315</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>316</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>317</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>318</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>319</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>320</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>321</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>322</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>323</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>324</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>325</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>326</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>327</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>328</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -8622,7 +8619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F336EB3-AE15-435C-BFD5-7698A0145ECB}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
@@ -8942,7 +8939,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B24" s="242" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C24" s="243"/>
       <c r="D24" s="243"/>
@@ -9171,7 +9168,7 @@
         <v>84</v>
       </c>
       <c r="D42" s="130" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E42" s="267" t="e">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D42, E$39, $D$29, , $D$32, $D$34, $D$35)*E40/100</f>
@@ -9595,7 +9592,7 @@
     </row>
     <row r="66" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B66" s="116" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E66" s="284"/>
       <c r="F66" s="284"/>
@@ -9648,7 +9645,7 @@
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B69" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D69" s="275" t="e" cm="1">
         <f t="array" ref="D69">INDEX(IS!21:21,MATCH(D$54,IS!$19:$19,0))/INDEX(IS!21:21,MATCH(D$54,IS!$19:$19,0)-1)-1</f>
@@ -9661,7 +9658,7 @@
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B70" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D70" s="276" t="e">
         <f>-D57/D56</f>
@@ -9674,7 +9671,7 @@
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B71" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D71" s="276"/>
       <c r="E71" s="289"/>
@@ -9684,7 +9681,7 @@
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B72" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D72" s="276"/>
       <c r="E72" s="280"/>
@@ -9694,7 +9691,7 @@
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B73" s="34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="276" t="e">
@@ -9708,7 +9705,7 @@
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B74" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="276" t="e">
@@ -9722,7 +9719,7 @@
     </row>
     <row r="75" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B75" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="277" t="e">

</xml_diff>

<commit_message>
bug fixes to form
</commit_message>
<xml_diff>
--- a/content/dcf_model_blank.xlsx
+++ b/content/dcf_model_blank.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeung\Documents\Programming\cash-flow-v3\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177A32F4-5ADC-444D-8B17-002768426C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457566AA-3747-4686-AAFF-B37AFF1D87CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="1000" activeTab="5" xr2:uid="{0646DCF6-9E5E-439A-8C31-869D606F0004}"/>
+    <workbookView xWindow="-28920" yWindow="7710" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="1" activeTab="1" xr2:uid="{0646DCF6-9E5E-439A-8C31-869D606F0004}"/>
   </bookViews>
   <sheets>
-    <sheet name="Assumptions" sheetId="272" r:id="rId1"/>
-    <sheet name="Output &gt;" sheetId="9" r:id="rId2"/>
-    <sheet name="DCF" sheetId="163" r:id="rId3"/>
-    <sheet name="Analysis &gt;" sheetId="269" r:id="rId4"/>
-    <sheet name="Discount rate" sheetId="166" r:id="rId5"/>
-    <sheet name="Beta" sheetId="167" r:id="rId6"/>
-    <sheet name="Comps" sheetId="270" r:id="rId7"/>
-    <sheet name="_CIQHiddenCacheSheet" sheetId="327" state="veryHidden" r:id="rId8"/>
+    <sheet name="_CIQHiddenCacheSheet" sheetId="329" state="veryHidden" r:id="rId1"/>
+    <sheet name="Assumptions" sheetId="272" r:id="rId2"/>
+    <sheet name="Output &gt;" sheetId="9" r:id="rId3"/>
+    <sheet name="DCF" sheetId="163" r:id="rId4"/>
+    <sheet name="Analysis &gt;" sheetId="269" r:id="rId5"/>
+    <sheet name="Discount rate" sheetId="166" r:id="rId6"/>
+    <sheet name="Beta" sheetId="167" r:id="rId7"/>
+    <sheet name="Comps" sheetId="270" r:id="rId8"/>
     <sheet name="Forecasts" sheetId="267" r:id="rId9"/>
     <sheet name="Data &gt;" sheetId="93" r:id="rId10"/>
     <sheet name="IS" sheetId="265" r:id="rId11"/>
@@ -34,7 +34,7 @@
     <definedName name="betaDate">Assumptions!$D$34</definedName>
     <definedName name="betaFreq">Assumptions!$D$36</definedName>
     <definedName name="ciqId">Assumptions!$D$9</definedName>
-    <definedName name="CIQWBGuid" hidden="1">"1c008d2a-84f6-4b5f-a676-b9a192bfcf13"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"a8276a67-f0b8-4891-a84e-adf74b8b0881"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.45.614.5792"" }"</definedName>
     <definedName name="convMode">Assumptions!$D$17</definedName>
     <definedName name="curr">Assumptions!$D$11</definedName>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="324">
   <si>
     <t>Risk free rate</t>
   </si>
@@ -1018,109 +1018,91 @@
     <t>Fixed operating costs</t>
   </si>
   <si>
-    <t>BAABTAVMT0NBTAFI/////wFQ/gAAACFDSVEuMC5JUV9FQklUREEuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCMiAcROBXtkIGUNJUS4uSVFfQ1VTVE9NX0JFVEEuLi4uLi4FAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIGkNJUS4uSVFfQ1VTVE9NX0JFVEEuLi4uLi4wBQAAAAEAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpDHlYE4Fe2QgMeVgTgV7ZCBtDSVEuLklRX0NVU1RPTV9CRVRBLi4uLi4wLjAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIHENJUS4uSVFfQ1VTVE9NX0JFVEEuLi4uMC4wLjAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIHUNJUS4uSVFfQ1VTVE9NX0JFVEEuLi5XLjAuMC4wBQAAAAEAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpDHlYE4Fe2QgMeVgTgV7ZCC9DSVEuLklRX0NVU1RPTV9CRVRBLjMxLzEyLzM3OTcuMDA6MDA6MDAuVy4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkIiAtxE4Fe2QggQ0lRLi5JUV9UT1RBTF9ERUJULi4wMDowMDowMC4uLi4FAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIIUNJUS4u</t>
-  </si>
-  <si>
-    <t>SVFfVE9UQUxfREVCVC4uMDA6MDA6MDAuLi4uMAUAAAABAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkIDHlYE4Fe2QgiQ0lRLi5JUV9UT1RBTF9ERUJULi4wMDowMDowMC4uLjAuMAUAAAABAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkIDHlYE4Fe2QgjQ0lRLi5JUV9UT1RBTF9ERUJULi4wMDowMDowMC4uMC4wLjAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIJENJUS4uSVFfVE9UQUxfREVCVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkIyIBxE4Fe2QglQ0lRLi5JUV9QUkVGX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkITZZwE4Fe2QgUQ0lRLi5JUV9NQVJLRVRDQVAuLi4FAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIHENJUS4uSVFfTUFSS0VUQ0FQLi4uMDA6MDA6MDAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCAx5WBOBXtkIJENJUS4uSVFfTUFSS0VUQ0FQLi4wMDowMDowMC4wMDowMDowMAUAAAABAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkIDHlYE4Fe2QgsQ0lRLi5JUV9NQVJLRVRDQVAuMDA6MDA6MDAu</t>
-  </si>
-  <si>
-    <t>MDA6MDA6MDAuMDA6MDA6MDAFAAAAAAAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCOMUdhOBXtkIFENJUS4uSVFfQ09NUEFOWV9OQU1FBQAAAAAAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpDHlYE4Fe2Qj39XETgV7ZCC5DSVEuLklRX0JVU0lORVNTX0RFU0NSSVBUSU9OLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpDHlYE4Fe2QiIC3ETgV7ZCCRDSVEuLklRX0NBU0hfRVFVSVYuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcikMeVgTgV7ZCMiAcROBXtkIJ0NJUS4uSVFfRkxPQVRfUEVSQ0VOVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkI9/VxE4Fe2QglQ0lRQVZHLi5JUV9WT0xVTUUuMzEvMTIvMzc5Ny4wMDowMDowMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkILWtyE4Fe2QgiQ0lRLi5JUV9URVZfRUJJVERBLklRX0xUTS4wMDowMDowMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkITZZwE4Fe2QgnQ0lRLjAuSVFfRUJJVERBLklRX0xUTS4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QiIC3ETgV7ZCCJDSVEuMC5J</t>
-  </si>
-  <si>
-    <t>UV9TVF9ERUJULi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2Qg4knITgV7ZCCJDSVEuMC5JUV9MVF9ERUJULi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QgCHXITgV7ZCCVDSVEuMC5JUV9DQVNIX0VRVUlWLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2Qj39XETgV7ZCCNDSVEuLklRX1dPUktJTkdfQ0FQLklRX0xUTS4wMDowMDowMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKQx5WBOBXtkILWtyE4Fe2QghQ0lRLi5JUV9UT1RBTF9SRVYuSVFfTFRNLjAwOjAwOjAwBQAAAAAAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpDHlYE4Fe2QhNlnATgV7ZCCtDSVEuMC5JUV9SRVZFTlVFX0VTVC5GWTE5MDAuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKQx5WBOBXtkI9zt2E4Fe2QgrQ0lRLjAuSVFfUkVWRU5VRV9FU1QuRlkxOTAxLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSkMeVgTgV7ZCPf1cROBXtkIK0NJUS4wLklRX1JFVkVOVUVfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKElu</t>
-  </si>
-  <si>
-    <t>dmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2Qj3O3YTgV7ZCDBDSVEuMC5JUV9HUk9TU19NQVJHSU5fRVNULkZZMTkwMC4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2Qh7TXcTgV7ZCDBDSVEuMC5JUV9HUk9TU19NQVJHSU5fRVNULkZZMTkwMS4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2QjjFHYTgV7ZCDBDSVEuMC5JUV9HUk9TU19NQVJHSU5fRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2QgVY3YTgV7ZCChDSVEuMC5JUV9FQklUX0VTVC5GWTE5MDAuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKQx5WBOBXtkI9zt2E4Fe2QgoQ0lRLjAuSVFfRUJJVF9FU1QuRlkxOTAxLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSkMeVgTgV7ZCE2WcBOBXtkIKENJUS4wLklRX0VCSVRfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2QgVY3YTgV7ZCCpDSVEuMC5JUV9FQklUREFfRVNULkZZMTkwMC4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUp</t>
-  </si>
-  <si>
-    <t>DHlYE4Fe2Qj3O3YTgV7ZCCpDSVEuMC5JUV9FQklUREFfRVNULkZZMTkwMS4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2QjIgHETgV7ZCCpDSVEuMC5JUV9FQklUREFfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2QgVY3YTgV7ZCCZDSVEuMC5JUV9EQV9FU1QuRlkxOTAwLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSkMeVgTgV7ZCPc7dhOBXtkIJkNJUS4wLklRX0RBX0VTVC5GWTE5MDEuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKQx5WBOBXtkI9/VxE4Fe2QgmQ0lRLjAuSVFfREFfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2Qj3O3YTgV7ZCClDSVEuMC5JUV9DQVBFWF9FU1QuRlkxOTAwLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSkMeVgTgV7ZCPc7dhOBXtkIKUNJUS4wLklRX0NBUEVYX0VTVC5GWTE5MDEuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKQx5WBOBXtkIlTJxE4Fe2QgpQ0lRLjAuSVFfQ0FQRVhfRVNULkZZMTkwMi4w</t>
-  </si>
-  <si>
-    <t>MDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpDHlYE4Fe2QgVY3YTgV7ZCCRDSVEuMC5JUV9UT1RBTF9SRVYuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCMiAcROBXtkIJkNJUS4wLklRX1RPVEFMX1JFVi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QgP/dMTgV7ZCCZDSVEuMC5JUV9UT1RBTF9SRVYuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI6K7TE4Fe2QgfQ0lRLjAuSVFfQ09HUy4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI9/VxE4Fe2QghQ0lRLjAuSVFfQ09HUy4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QiJDtUTgV7ZCCFDSVEuMC5JUV9DT0dTLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCGHA1BOBXtkIHkNJUS4wLklRX1NHQS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5</t>
-  </si>
-  <si>
-    <t>WBOBXtkIyIBxE4Fe2QggQ0lRLjAuSVFfU0dBLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCGHA1BOBXtkIIENJUS4wLklRX1NHQS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QhactQTgV7ZCCFDSVEuMC5JUV9SRF9FWFAuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCPf1cROBXtkII0NJUS4wLklRX1JEX0VYUC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QjortMTgV7ZCCNDSVEuMC5JUV9SRF9FWFAuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIKkvUE4Fe2QglQ0lRLjAuSVFfT1RIRVJfT1BFUi4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkITZZwE4Fe2QgnQ0lRLjAuSVFfT1RIRVJfT1BFUi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QhhwNQTgV7ZCCdDSVEuMC5JUV9PVEhFUl9PUEVSLi4zMS8xMi8xOTAx</t>
-  </si>
-  <si>
-    <t>LjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCIkO1ROBXtkIHUNJUS4wLklRX0RBLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QiIC3ETgV7ZCB9DSVEuMC5JUV9EQS4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QhactQTgV7ZCB9DSVEuMC5JUV9EQS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QgP/dMTgV7ZCCdDSVEuMC5JUV9JTlRFUkVTVF9FWFAuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCB5EchOBXtkIKUNJUS4wLklRX0lOVEVSRVNUX0VYUC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QgP/dMTgV7ZCClDSVEuMC5JUV9JTlRFUkVTVF9FWFAuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIiQ7VE4Fe2QguQ0lRLjAuSVFfSU5URVJFU1RfSU5WRVNUX0lOQy4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBS</t>
-  </si>
-  <si>
-    <t>ZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIXL1wE4Fe2QgwQ0lRLjAuSVFfSU5URVJFU1RfSU5WRVNUX0lOQy4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QiJDtUTgV7ZCDBDSVEuMC5JUV9JTlRFUkVTVF9JTlZFU1RfSU5DLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCFOZ1BOBXtkIKENJUS4wLklRX0NVUlJFTkNZX0dBSU4uLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCKhZcROBXtkIKkNJUS4wLklRX0NVUlJFTkNZX0dBSU4uLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkID/3TE4Fe2QgqQ0lRLjAuSVFfQ1VSUkVOQ1lfR0FJTi4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QjortMTgV7ZCDNDSVEuMC5JUV9PVEhFUl9OT05fT1BFUl9FWFBfU1VQUEwuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCMiAcROBXtkINUNJUS4wLklRX09USEVSX05PTl9PUEVSX0VYUF9TVVBQTC4uMzEvMTIv</t>
-  </si>
-  <si>
-    <t>MTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QjortMTgV7ZCDVDSVEuMC5JUV9PVEhFUl9OT05fT1BFUl9FWFBfU1VQUEwuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI0IfTE4Fe2QgeQ0lRLjAuSVFfRUJULi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2Qg8b3ATgV7ZCCBDSVEuMC5JUV9FQlQuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIU5nUE4Fe2QggQ0lRLjAuSVFfRUJULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCFpy1BOBXtkIIkNJUS4wLklRX0lOQ19UQVguLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCN7OcROBXtkIJENJUS4wLklRX0lOQ19UQVguLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI6K7TE4Fe2QgkQ0lRLjAuSVFfSU5DX1RBWC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJl</t>
-  </si>
-  <si>
-    <t>c3RhdGVtZW50IFR5cGUpDHlYE4Fe2QiJDtUTgV7ZCB1DSVEuMC5JUV9OSS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIduRwE4Fe2QgfQ0lRLjAuSVFfTkkuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIWnLUE4Fe2QgfQ0lRLjAuSVFfTkkuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkID/3TE4Fe2QgnQ0lRLjAuSVFfQ0FTSF9FUVVJVi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QiUNdUTgV7ZCCdDSVEuMC5JUV9DQVNIX0VRVUlWLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCGHA1BOBXtkIJENJUS4wLklRX1NUX0lOVkVTVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIqFlxE4Fe2QgmQ0lRLjAuSVFfU1RfSU5WRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCBYk1BOBXtkIJkNJUS4wLklRX1NUX0lO</t>
-  </si>
-  <si>
-    <t>VkVTVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2Qj61dMTgV7ZCB1DSVEuMC5JUV9BUi4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkILWtyE4Fe2QgfQ0lRLjAuSVFfQVIuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI6K7TE4Fe2QgfQ0lRLjAuSVFfQVIuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI6K7TE4Fe2QgnQ0lRLjAuSVFfT1RIRVJfUkVDRUlWLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2Qg8b3ATgV7ZCClDSVEuMC5JUV9PVEhFUl9SRUNFSVYuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIYcDUE4Fe2QgpQ0lRLjAuSVFfT1RIRVJfUkVDRUlWLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCFpy1BOBXtkIJENJUS4wLklRX0lOVkVOVE9SWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52</t>
-  </si>
-  <si>
-    <t>YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkI3s5xE4Fe2QgmQ0lRLjAuSVFfSU5WRU5UT1JZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCPrV0xOBXtkIJkNJUS4wLklRX0lOVkVOVE9SWS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QgWJNQTgV7ZCCpDSVEuMC5JUV9SRVNUUklDVEVEX0NBU0guLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCB5EchOBXtkILENJUS4wLklRX1JFU1RSSUNURURfQ0FTSC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpDHlYE4Fe2QhactQTgV7ZCCxDSVEuMC5JUV9SRVNUUklDVEVEX0NBU0guLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIlDXVE4Fe2QgjQ0lRLjAuSVFfVE9UQUxfQ0EuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCHbkcBOBXtkIJUNJUS4wLklRX1RPVEFMX0NBLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0</t>
-  </si>
-  <si>
-    <t>ZW1lbnQgVHlwZSkMeVgTgV7ZCFOZ1BOBXtkIJUNJUS4wLklRX1RPVEFMX0NBLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCBYk1BOBXtkIH0NJUS4wLklRX05QUEUuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkMeVgTgV7ZCKhZcROBXtkIIUNJUS4wLklRX05QUEUuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKQx5WBOBXtkIFiTUE4Fe2QghQ0lRLjAuSVFfTlBQRS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QjortMTgV7ZCB1DSVEuMC5JUV9HVy4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIXL1wE4Fe2QgfQ0lRLjAuSVFfR1cuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIlDXVE4Fe2QgfQ0lRLjAuSVFfR1cuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIYcDUE4Fe2QgmQ0lRLjAuSVFfT1RIRVJfSU5UQU4uLjAwOjAwOjAwLjAuMC4w</t>
-  </si>
-  <si>
-    <t>LjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCKhZcROBXtkIKENJUS4wLklRX09USEVSX0lOVEFOLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCGHA1BOBXtkIKENJUS4wLklRX09USEVSX0lOVEFOLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCFOZ1BOBXtkIJENJUS4wLklRX0xUX0lOVkVTVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkI3s5xE4Fe2QgmQ0lRLjAuSVFfTFRfSU5WRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCOiu0xOBXtkIJkNJUS4wLklRX0xUX0lOVkVTVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QjQh9MTgV7ZCCdDSVEuMC5JUV9UT1RBTF9BU1NFVFMuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCDxvcBOBXtkIKUNJUS4wLklRX1RPVEFMX0FTU0VUUy4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJ</t>
-  </si>
-  <si>
-    <t>bnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QhhwNQTgV7ZCClDSVEuMC5JUV9UT1RBTF9BU1NFVFMuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIiQ7VE4Fe2QgdQ0lRLjAuSVFfQVAuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCHbkcBOBXtkIH0NJUS4wLklRX0FQLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCFOZ1BOBXtkIH0NJUS4wLklRX0FQLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCBYk1BOBXtkIHUNJUS4wLklRX0FFLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QgeRHITgV7ZCB9DSVEuMC5JUV9BRS4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QjQh9MTgV7ZCB9DSVEuMC5JUV9BRS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QiUNdUTgV7ZCCRDSVEuMC5JUV9TVF9ERUJULi4zMS8xMi8x</t>
-  </si>
-  <si>
-    <t>OTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCKlc1ROBXtkIJENJUS4wLklRX1NUX0RFQlQuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIcefUE4Fe2QgsQ0lRLjAuSVFfQ1VSUkVOVF9QT1JUX0RFQlQuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCKhZcROBXtkILkNJUS4wLklRX0NVUlJFTlRfUE9SVF9ERUJULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCCpL1BOBXtkILkNJUS4wLklRX0NVUlJFTlRfUE9SVF9ERUJULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCA/90xOBXtkILkNJUS4wLklRX0NVUlJFTlRfUE9SVF9MRUFTRVMuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCDiSchOBXtkIMENJUS4wLklRX0NVUlJFTlRfUE9SVF9MRUFTRVMuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkI+tXTE4Fe2QgwQ0lRLjAuSVFfQ1VS</t>
-  </si>
-  <si>
-    <t>UkVOVF9QT1JUX0xFQVNFUy4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QgP/dMTgV7ZCC1DSVEuMC5JUV9VTkVBUk5fUkVWX0NVUlJFTlQuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCDxvcBOBXtkIL0NJUS4wLklRX1VORUFSTl9SRVZfQ1VSUkVOVC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2Qhx59QTgV7ZCC9DSVEuMC5JUV9VTkVBUk5fUkVWX0NVUlJFTlQuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIU5nUE4Fe2QgjQ0lRLjAuSVFfVE9UQUxfQ0wuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCM6ncROBXtkIJUNJUS4wLklRX1RPVEFMX0NMLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCPrV0xOBXtkIJUNJUS4wLklRX1RPVEFMX0NMLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCCpL1BOBXtkIJENJUS4w</t>
-  </si>
-  <si>
-    <t>LklRX0xUX0RFQlQuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIiQ7VE4Fe2QgkQ0lRLjAuSVFfTFRfREVCVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QipXNUTgV7ZCCtDSVEuMC5JUV9MT05HX1RFUk1fTEVBU0VTLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2Qh25HATgV7ZCC1DSVEuMC5JUV9MT05HX1RFUk1fTEVBU0VTLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCFOZ1BOBXtkILUNJUS4wLklRX0xPTkdfVEVSTV9MRUFTRVMuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIKkvUE4Fe2QgoQ0lRLjAuSVFfVU5FQVJOX1JFVl9MVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIlTJxE4Fe2QgqQ0lRLjAuSVFfVU5FQVJOX1JFVl9MVC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QgqS9QTgV7ZCCpDSVEuMC5J</t>
-  </si>
-  <si>
-    <t>UV9VTkVBUk5fUkVWX0xULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCPrV0xOBXtkIKkNJUS4wLklRX0RFRl9UQVhfTElBQl9MVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIyIBxE4Fe2QgsQ0lRLjAuSVFfREVGX1RBWF9MSUFCX0xULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCKlc1ROBXtkILENJUS4wLklRX0RFRl9UQVhfTElBQl9MVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2Qhx59QTgV7ZCCVDSVEuMC5JUV9UT1RBTF9MSUFCLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QiVMnETgV7ZCCdDSVEuMC5JUV9UT1RBTF9MSUFCLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCHHn1BOBXtkIJ0NJUS4wLklRX1RPVEFMX0xJQUIuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIWnLUE4Fe2QghQ0lRLjAuSVFf</t>
-  </si>
-  <si>
-    <t>Q09NTU9OLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QjOp3ETgV7ZCCNDSVEuMC5JUV9DT01NT04uLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkI+tXTE4Fe2QgjQ0lRLjAuSVFfQ09NTU9OLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCNCH0xOBXtkIH0NJUS4wLklRX0FQSUMuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCC9IcBOBXtkIIUNJUS4wLklRX0FQSUMuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIcefUE4Fe2QghQ0lRLjAuSVFfQVBJQy4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QiUNdUTgV7ZCB1DSVEuMC5JUV9SRS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIXL1wE4Fe2QgfQ0lRLjAuSVFfUkUuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBl</t>
-  </si>
-  <si>
-    <t>KR+gWBOBXtkIWnLUE4Fe2QgfQ0lRLjAuSVFfUkUuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIKkvUE4Fe2QgjQ0lRLjAuSVFfVFJFQVNVUlkuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCAIdchOBXtkIJUNJUS4wLklRX1RSRUFTVVJZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCNCH0xOBXtkIJUNJUS4wLklRX1RSRUFTVVJZLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCJQ11ROBXtkIJ0NJUS4wLklRX09USEVSX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkI9/VxE4Fe2QgpQ0lRLjAuSVFfT1RIRVJfRVFVSVRZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCJQ11ROBXtkIKUNJUS4wLklRX09USEVSX0VRVUlUWS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2Qhx59QTgV7ZCCZDSVEuMC5JUV9Q</t>
-  </si>
-  <si>
-    <t>UkVGX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIlTJxE4Fe2QgoQ0lRLjAuSVFfUFJFRl9FUVVJVFkuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIFiTUE4Fe2QgoQ0lRLjAuSVFfUFJFRl9FUVVJVFkuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkI+tXTE4Fe2QgsQ0lRLjAuSVFfTUlOT1JJVFlfSU5URVJFU1QuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCC1rchOBXtkILkNJUS4wLklRX01JTk9SSVRZX0lOVEVSRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCJQ11ROBXtkILkNJUS4wLklRX01JTk9SSVRZX0lOVEVSRVNULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCGHA1BOBXtkIJ0NJUS4wLklRX1RPVEFMX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIlTJxE4Fe2QgpQ0lRLjAu</t>
-  </si>
-  <si>
-    <t>SVFfVE9UQUxfRVFVSVRZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCBYk1BOBXtkIKUNJUS4wLklRX1RPVEFMX0VRVUlUWS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2Qj61dMTgV7ZCCRDSVEuMC5JUV9DQVNIX09QRVIuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCC1rchOBXtkIJkNJUS4wLklRX0NBU0hfT1BFUi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QipXNUTgV7ZCCZDSVEuMC5JUV9DQVNIX09QRVIuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIiQ7VE4Fe2QgmQ0lRLjAuSVFfQ0FTSF9JTlZFU1QuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCJUycROBXtkIKENJUS4wLklRX0NBU0hfSU5WRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCCpL1BOBXtkIKENJUS4wLklRX0NBU0hfSU5WRVNULi4z</t>
-  </si>
-  <si>
-    <t>MS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCA/90xOBXtkIJUNJUS4wLklRX0NBU0hfRklOQU4uLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCMiAcROBXtkIJ0NJUS4wLklRX0NBU0hfRklOQU4uLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkID/3TE4Fe2QgnQ0lRLjAuSVFfQ0FTSF9GSU5BTi4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QjortMTgV7ZCCVDSVEuMC5JUV9ORVRfQ0hBTkdFLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QgvSHATgV7ZCCdDSVEuMC5JUV9ORVRfQ0hBTkdFLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCPMJ1ROBXtkIJ0NJUS4wLklRX05FVF9DSEFOR0UuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKR+gWBOBXtkIU5nUE4Fe2QggQ0lRLjAuSVFfQ0FQRVguLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgA</t>
-  </si>
-  <si>
-    <t>AAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCM6ncROBXtkIIkNJUS4wLklRX0NBUEVYLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCA/90xOBXtkIIkNJUS4wLklRX0NBUEVYLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSkfoFgTgV7ZCKlc1ROBXtkILENJUS4wLklRX1RPVEFMX0RJVl9QQUlEX0NGLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QhcvXATgV7ZCC5DSVEuMC5JUV9UT1RBTF9ESVZfUEFJRF9DRi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QhTmdQTgV7ZCC5DSVEuMC5JUV9UT1RBTF9ESVZfUEFJRF9DRi4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpH6BYE4Fe2QgqS9QTgV7ZCCJDSVEuMC5JUV9FQklUX0VTVC4uMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKY9T+iqAXtkIiAtxE4Fe2QgqQ0lRLjAuSVFfR1JPU1NfTUFSR0lOX0VTVC4uMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZp</t>
-  </si>
-  <si>
-    <t>bGluZyBNb2RlKY9T+iqAXtkILWtyE4Fe2QggQ0lRLjAuSVFfREFfRVNULi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpj1P6KoBe2Qgta3ITgV7ZCCRDSVEuMC5JUV9FQklUREFfRVNULi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpj1P6KoBe2QjIgHETgV7ZCCNDSVEuMC5JUV9DQVBFWF9FU1QuLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSmPU/oqgF7ZCC1rchOBXtkIJUNJUS4wLklRX1JFVkVOVUVfRVNULi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpj1P6KoBe2Qgta3ITgV7ZCBhDSVEuMC5JUV9DQVBFWC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIHENJUS4wLklRX0NBU0hfT1BFUi4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIJENJUS4wLklRX01JTk9SSVRZX0lOVEVSRVNULi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgfQ0lRLjAuSVFfT1RIRVJfRVFVSVRZLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBS</t>
-  </si>
-  <si>
-    <t>ZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgXQ0lRLjAuSVFfQVBJQy4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIG0NJUS4wLklRX1RSRUFTVVJZLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgiQ0lRLjAuSVFfREVGX1RBWF9MSUFCX0xULi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgaQ0lRLjAuSVFfTFRfREVCVC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIGkNJUS4wLklRX1NUX0RFQlQuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCB9DSVEuMC5JUV9UT1RBTF9BU1NFVFMuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBVDSVEuMC5JUV9BRS4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIFUNJUS4wLklRX0dXLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkI</t>
-  </si>
-  <si>
-    <t>ymvEE4Fe2QgiQ0lRLjAuSVFfUkVTVFJJQ1RFRF9DQVNILi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgdQ0lRLjAuSVFfQ0FTSF9FUVVJVi4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIGkNJUS4wLklRX0lOQ19UQVguLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCCZDSVEuMC5JUV9JTlRFUkVTVF9JTlZFU1RfSU5DLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgdQ0lRLjAuSVFfT1RIRVJfT1BFUi4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIH0NJUS4wLklRX0lOVEVSRVNUX0VYUC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIF0NJUS4wLklRX0NPR1MuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCB1DSVEuMC5JUV9ORVRfQ0hBTkdFLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcpr</t>
-  </si>
-  <si>
-    <t>xBOBXtkIymvEE4Fe2QgdQ0lRLjAuSVFfVE9UQUxfTElBQi4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIJUNJUS4wLklRX1VORUFSTl9SRVZfQ1VSUkVOVC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIHkNJUS4wLklRX09USEVSX0lOVEFOLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgfQ0lRLjAuSVFfT1RIRVJfUkVDRUlWLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgWQ0lRLjAuSVFfRUJULi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgWQ0lRLjAuSVFfU0dBLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgkQ0lRLjAuSVFfVE9UQUxfRElWX1BBSURfQ0YuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBVDSVEuMC5JUV9SRS4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7Z</t>
-  </si>
-  <si>
-    <t>CMprxBOBXtkII0NJUS4wLklRX0xPTkdfVEVSTV9MRUFTRVMuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBVDSVEuMC5JUV9BUC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIG0NJUS4wLklRX1RPVEFMX0NBLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgVQ0lRLjAuSVFfTkkuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBVDSVEuMC5JUV9EQS4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIGUNJUS4wLklRX1JEX0VYUC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIHkNJUS4wLklRX0NBU0hfSU5WRVNULi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgfQ0lRLjAuSVFfVE9UQUxfRVFVSVRZLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgeQ0lRLjAuSVFfUFJF</t>
-  </si>
-  <si>
-    <t>Rl9FUVVJVFkuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCCBDSVEuMC5JUV9VTkVBUk5fUkVWX0xULi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgbQ0lRLjAuSVFfVE9UQUxfQ0wuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCCRDSVEuMC5JUV9DVVJSRU5UX1BPUlRfREVCVC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIF0NJUS4wLklRX05QUEUuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBxDSVEuMC5JUV9JTlZFTlRPUlkuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBxDSVEuMC5JUV9TVF9JTlZFU1QuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCCBDSVEuMC5JUV9DVVJSRU5DWV9HQUlOLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgcQ0lRLjAuSVFf</t>
-  </si>
-  <si>
-    <t>VE9UQUxfUkVWLi4uMC4wLjAuMAUAAAABAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKcprxBOBXtkIymvEE4Fe2QgmQ0lRLjAuSVFfQ1VSUkVOVF9QT1JUX0xFQVNFUy4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIHUNJUS4wLklRX0NBU0hfRklOQU4uLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBlDSVEuMC5JUV9DT01NT04uLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBxDSVEuMC5JUV9MVF9JTlZFU1QuLi4wLjAuMC4wBQAAAAEAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpymvEE4Fe2QjKa8QTgV7ZCBVDSVEuMC5JUV9BUi4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkIK0NJUS4wLklRX09USEVSX05PTl9PUEVSX0VYUF9TVVBQTC4uLjAuMC4wLjAFAAAAAQAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnKa8QTgV7ZCMprxBOBXtkI</t>
-  </si>
-  <si>
     <t>Note: Please input corporate tax rates.</t>
+  </si>
+  <si>
+    <t>BAABTAVMT0NBTAFI/////wFQywAAACFDSVEuMC5JUV9FQklUREEuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSm2fHm3LWDZCJK7mrctYNkIGUNJUS4uSVFfQ1VTVE9NX0JFVEEuLi4uLi4FAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcim/o3m3LWDZCL+jebctYNkIGkNJUS4uSVFfQ1VTVE9NX0JFVEEuLi4uLi4wBQAAAAEAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpv6N5ty1g2Qi/o3m3LWDZCBtDSVEuLklRX0NVU1RPTV9CRVRBLi4uLi4wLjAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcim/o3m3LWDZCL+jebctYNkIHENJUS4uSVFfQ1VTVE9NX0JFVEEuLi4uMC4wLjAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCMzKebctYNkIHUNJUS4uSVFfQ1VTVE9NX0JFVEEuLi5XLjAuMC4wBQAAAAEAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpzMp5ty1g2QjMynm3LWDZCC9DSVEuLklRX0NVU1RPTV9CRVRBLjMxLzEyLzM3OTcuMDA6MDA6MDAuVy4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIXUaaty1g2QggQ0lRLi5JUV9UT1RBTF9ERUJULi4wMDowMDowMC4uLi4FAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCMzKebctYNkIIUNJUS4u</t>
+  </si>
+  <si>
+    <t>SVFfVE9UQUxfREVCVC4uMDA6MDA6MDAuLi4uMAUAAAABAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIzMp5ty1g2QgiQ0lRLi5JUV9UT1RBTF9ERUJULi4wMDowMDowMC4uLjAuMAUAAAABAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIzMp5ty1g2QgjQ0lRLi5JUV9UT1RBTF9ERUJULi4wMDowMDowMC4uMC4wLjAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCMzKebctYNkIJENJUS4uSVFfVE9UQUxfREVCVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIOfiZty1g2QglQ0lRLi5JUV9QUkVGX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIJ9GZty1g2QgUQ0lRLi5JUV9NQVJLRVRDQVAuLi4FAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCMzKebctYNkIHENJUS4uSVFfTUFSS0VUQ0FQLi4uMDA6MDA6MDAFAAAAAQAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCMzKebctYNkIJENJUS4uSVFfTUFSS0VUQ0FQLi4wMDowMDowMC4wMDowMDowMAUAAAABAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIzMp5ty1g2QgsQ0lRLi5JUV9NQVJLRVRDQVAuMDA6MDA6MDAu</t>
+  </si>
+  <si>
+    <t>MDA6MDA6MDAuMDA6MDA6MDAFAAAAAAAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCF1GmrctYNkIFENJUS4uSVFfQ09NUEFOWV9OQU1FBQAAAAAAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpzMp5ty1g2Qj6pZu3LWDZCC5DSVEuLklRX0JVU0lORVNTX0RFU0NSSVBUSU9OLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpzMp5ty1g2QhdRpq3LWDZCCRDSVEuLklRX0NBU0hfRVFVSVYuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAUKEludmFsaWQgSWRlbnRpZmllcinMynm3LWDZCJK7mrctYNkIJ0NJUS4uSVFfRkxPQVRfUEVSQ0VOVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIswmbty1g2QglQ0lRQVZHLi5JUV9WT0xVTUUuMzEvMTIvMzc5Ny4wMDowMDowMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkI+qWbty1g2QgiQ0lRLi5JUV9URVZfRUJJVERBLklRX0xUTS4wMDowMDowMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIXUaaty1g2QgnQ0lRLjAuSVFfRUJJVERBLklRX0xUTS4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhvbZq3LWDZCCJDSVEuMC5J</t>
+  </si>
+  <si>
+    <t>UV9TVF9ERUJULi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QizCZu3LWDZCCJDSVEuMC5JUV9MVF9ERUJULi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QjaV5u3LWDZCCVDSVEuMC5JUV9DQVNIX0VRVUlWLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qj6pZu3LWDZCCNDSVEuLklRX1dPUktJTkdfQ0FQLklRX0xUTS4wMDowMDowMAUAAAAAAAAACAAAABQoSW52YWxpZCBJZGVudGlmaWVyKczKebctYNkIJ9GZty1g2QghQ0lRLi5JUV9UT1RBTF9SRVYuSVFfTFRNLjAwOjAwOjAwBQAAAAAAAAAIAAAAFChJbnZhbGlkIElkZW50aWZpZXIpzMp5ty1g2Qgn0Zm3LWDZCCtDSVEuMC5JUV9SRVZFTlVFX0VTVC5GWTE5MDAuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKczKebctYNkIyKnSty1g2QgrQ0lRLjAuSVFfUkVWRU5VRV9FU1QuRlkxOTAxLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSnMynm3LWDZCMowm7ctYNkIK0NJUS4wLklRX1JFVkVOVUVfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKElu</t>
+  </si>
+  <si>
+    <t>dmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2Qi3gtK3LWDZCDBDSVEuMC5JUV9HUk9TU19NQVJHSU5fRVNULkZZMTkwMC4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2QjIqdK3LWDZCDBDSVEuMC5JUV9HUk9TU19NQVJHSU5fRVNULkZZMTkwMS4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2Qj6pZu3LWDZCDBDSVEuMC5JUV9HUk9TU19NQVJHSU5fRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2Qi3gtK3LWDZCChDSVEuMC5JUV9FQklUX0VTVC5GWTE5MDAuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKczKebctYNkIt4LSty1g2QgoQ0lRLjAuSVFfRUJJVF9FU1QuRlkxOTAxLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSnMynm3LWDZCCfRmbctYNkIKENJUS4wLklRX0VCSVRfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2QjIqdK3LWDZCCpDSVEuMC5JUV9FQklUREFfRVNULkZZMTkwMC4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUp</t>
+  </si>
+  <si>
+    <t>zMp5ty1g2QjIqdK3LWDZCCpDSVEuMC5JUV9FQklUREFfRVNULkZZMTkwMS4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2QiSu5q3LWDZCCpDSVEuMC5JUV9FQklUREFfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2QjIqdK3LWDZCCZDSVEuMC5JUV9EQV9FU1QuRlkxOTAwLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSnMynm3LWDZCMip0rctYNkIJkNJUS4wLklRX0RBX0VTVC5GWTE5MDEuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKczKebctYNkIyjCbty1g2QgmQ0lRLjAuSVFfREFfRVNULkZZMTkwMi4wMDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2Qi3gtK3LWDZCClDSVEuMC5JUV9DQVBFWF9FU1QuRlkxOTAwLjAwOjAwOjAwLi4wLjAuMAUAAAAAAAAACAAAABUoSW52YWxpZCBGaWxpbmcgTW9kZSnMynm3LWDZCLeC0rctYNkIKUNJUS4wLklRX0NBUEVYX0VTVC5GWTE5MDEuMDA6MDA6MDAuLjAuMC4wBQAAAAAAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKczKebctYNkI+qWbty1g2QgpQ0lRLjAuSVFfQ0FQRVhfRVNULkZZMTkwMi4w</t>
+  </si>
+  <si>
+    <t>MDowMDowMC4uMC4wLjAFAAAAAAAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpzMp5ty1g2Qi3gtK3LWDZCCRDSVEuMC5JUV9UT1RBTF9SRVYuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIJkNJUS4wLklRX1RPVEFMX1JFVi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QizCZu3LWDZCCZDSVEuMC5JUV9UT1RBTF9SRVYuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI536bty1g2QgfQ0lRLjAuSVFfQ09HUy4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIyjCbty1g2QghQ0lRLjAuSVFfQ09HUy4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qgn0Zm3LWDZCCFDSVEuMC5JUV9DT0dTLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCF1GmrctYNkIHkNJUS4wLklRX1NHQS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczK</t>
+  </si>
+  <si>
+    <t>ebctYNkIkruaty1g2QggQ0lRLjAuSVFfU0dBLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCF1GmrctYNkIIENJUS4wLklRX1NHQS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qh+lJq3LWDZCCFDSVEuMC5JUV9SRF9FWFAuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCLMJm7ctYNkII0NJUS4wLklRX1JEX0VYUC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qjnfpu3LWDZCCNDSVEuMC5JUV9SRF9FWFAuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI2lebty1g2QglQ0lRLjAuSVFfT1RIRVJfT1BFUi4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIJ9GZty1g2QgnQ0lRLjAuSVFfT1RIRVJfT1BFUi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhdRpq3LWDZCCdDSVEuMC5JUV9PVEhFUl9PUEVSLi4zMS8xMi8xOTAx</t>
+  </si>
+  <si>
+    <t>LjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCCfRmbctYNkIHUNJUS4wLklRX0RBLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhMH5q3LWDZCB9DSVEuMC5JUV9EQS4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qh+lJq3LWDZCB9DSVEuMC5JUV9EQS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QizCZu3LWDZCCdDSVEuMC5JUV9JTlRFUkVTVF9FWFAuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCOd+m7ctYNkIKUNJUS4wLklRX0lOVEVSRVNUX0VYUC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhvbZq3LWDZCClDSVEuMC5JUV9JTlRFUkVTVF9FWFAuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIJ9GZty1g2QguQ0lRLjAuSVFfSU5URVJFU1RfSU5WRVNUX0lOQy4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBS</t>
+  </si>
+  <si>
+    <t>ZXN0YXRlbWVudCBUeXBlKczKebctYNkIXUaaty1g2QgwQ0lRLjAuSVFfSU5URVJFU1RfSU5WRVNUX0lOQy4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCDBDSVEuMC5JUV9JTlRFUkVTVF9JTlZFU1RfSU5DLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCEwfmrctYNkIKENJUS4wLklRX0NVUlJFTkNZX0dBSU4uLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIKkNJUS4wLklRX0NVUlJFTkNZX0dBSU4uLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIswmbty1g2QgqQ0lRLjAuSVFfQ1VSUkVOQ1lfR0FJTi4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qjnfpu3LWDZCDNDSVEuMC5JUV9PVEhFUl9OT05fT1BFUl9FWFBfU1VQUEwuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCDn4mbctYNkINUNJUS4wLklRX09USEVSX05PTl9PUEVSX0VYUF9TVVBQTC4uMzEvMTIv</t>
+  </si>
+  <si>
+    <t>MTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qjnfpu3LWDZCDVDSVEuMC5JUV9PVEhFUl9OT05fT1BFUl9FWFBfU1VQUEwuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIyjCbty1g2QgeQ0lRLjAuSVFfRUJULi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCCBDSVEuMC5JUV9FQlQuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkITB+aty1g2QggQ0lRLjAuSVFfRUJULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIIkNJUS4wLklRX0lOQ19UQVguLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCLMJm7ctYNkIJENJUS4wLklRX0lOQ19UQVguLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI536bty1g2QgkQ0lRLjAuSVFfSU5DX1RBWC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJl</t>
+  </si>
+  <si>
+    <t>c3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCB1DSVEuMC5JUV9OSS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkITB+aty1g2QgfQ0lRLjAuSVFfTkkuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIfpSaty1g2QgfQ0lRLjAuSVFfTkkuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIswmbty1g2QgnQ0lRLjAuSVFfQ0FTSF9FUVVJVi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCCdDSVEuMC5JUV9DQVNIX0VRVUlWLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCEwfmrctYNkIJENJUS4wLklRX1NUX0lOVkVTVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIfpSaty1g2QgmQ0lRLjAuSVFfU1RfSU5WRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCLMJm7ctYNkIJkNJUS4wLklRX1NUX0lO</t>
+  </si>
+  <si>
+    <t>VkVTVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qjnfpu3LWDZCB1DSVEuMC5JUV9BUi4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI2lebty1g2QgfQ0lRLjAuSVFfQVIuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI536bty1g2QgfQ0lRLjAuSVFfQVIuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIOfiZty1g2QgnQ0lRLjAuSVFfT1RIRVJfUkVDRUlWLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCClDSVEuMC5JUV9PVEhFUl9SRUNFSVYuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkITB+aty1g2QgpQ0lRLjAuSVFfT1RIRVJfUkVDRUlWLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIJENJUS4wLklRX0lOVkVOVE9SWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52</t>
+  </si>
+  <si>
+    <t>YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIneKaty1g2QgmQ0lRLjAuSVFfSU5WRU5UT1JZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCOd+m7ctYNkIJkNJUS4wLklRX0lOVkVOVE9SWS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qid4pq3LWDZCCpDSVEuMC5JUV9SRVNUUklDVEVEX0NBU0guLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCOd+m7ctYNkILENJUS4wLklRX1JFU1RSSUNURURfQ0FTSC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhdRpq3LWDZCCxDSVEuMC5JUV9SRVNUUklDVEVEX0NBU0guLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIC6qZty1g2QgjQ0lRLjAuSVFfVE9UQUxfQ0EuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCEwfmrctYNkIJUNJUS4wLklRX1RPVEFMX0NBLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0</t>
+  </si>
+  <si>
+    <t>ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIJUNJUS4wLklRX1RPVEFMX0NBLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCJ3imrctYNkIH0NJUS4wLklRX05QUEUuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIIUNJUS4wLklRX05QUEUuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIneKaty1g2QghQ0lRLjAuSVFfTlBQRS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qjnfpu3LWDZCB1DSVEuMC5JUV9HVy4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIyjCbty1g2QgfQ0lRLjAuSVFfR1cuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIC6qZty1g2QgfQ0lRLjAuSVFfR1cuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkITB+aty1g2QgmQ0lRLjAuSVFfT1RIRVJfSU5UQU4uLjAwOjAwOjAwLjAuMC4w</t>
+  </si>
+  <si>
+    <t>LjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIKENJUS4wLklRX09USEVSX0lOVEFOLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCEwfmrctYNkIKENJUS4wLklRX09USEVSX0lOVEFOLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIJENJUS4wLklRX0xUX0lOVkVTVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIneKaty1g2QgmQ0lRLjAuSVFfTFRfSU5WRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCOd+m7ctYNkIJkNJUS4wLklRX0xUX0lOVkVTVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qg5+Jm3LWDZCCdDSVEuMC5JUV9UT1RBTF9BU1NFVFMuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCAuqmbctYNkIKUNJUS4wLklRX1RPVEFMX0FTU0VUUy4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJ</t>
+  </si>
+  <si>
+    <t>bnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhMH5q3LWDZCClDSVEuMC5JUV9UT1RBTF9BU1NFVFMuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIC6qZty1g2QgdQ0lRLjAuSVFfQVAuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCEwfmrctYNkIH0NJUS4wLklRX0FQLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkIH0NJUS4wLklRX0FQLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCJ3imrctYNkIHUNJUS4wLklRX0FFLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qjnfpu3LWDZCB9DSVEuMC5JUV9BRS4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QjaV5u3LWDZCB9DSVEuMC5JUV9BRS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCCRDSVEuMC5JUV9TVF9ERUJULi4zMS8xMi8x</t>
+  </si>
+  <si>
+    <t>OTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCAuqmbctYNkIJENJUS4wLklRX1NUX0RFQlQuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkITB+aty1g2QgsQ0lRLjAuSVFfQ1VSUkVOVF9QT1JUX0RFQlQuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCH6UmrctYNkILkNJUS4wLklRX0NVUlJFTlRfUE9SVF9ERUJULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCJ3imrctYNkILkNJUS4wLklRX0NVUlJFTlRfUE9SVF9ERUJULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCOd+m7ctYNkILkNJUS4wLklRX0NVUlJFTlRfUE9SVF9MRUFTRVMuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCCfRmbctYNkIMENJUS4wLklRX0NVUlJFTlRfUE9SVF9MRUFTRVMuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI2lebty1g2QgwQ0lRLjAuSVFfQ1VS</t>
+  </si>
+  <si>
+    <t>UkVOVF9QT1JUX0xFQVNFUy4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhdRpq3LWDZCC1DSVEuMC5JUV9VTkVBUk5fUkVWX0NVUlJFTlQuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCAuqmbctYNkIL0NJUS4wLklRX1VORUFSTl9SRVZfQ1VSUkVOVC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhMH5q3LWDZCC9DSVEuMC5JUV9VTkVBUk5fUkVWX0NVUlJFTlQuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QgjQ0lRLjAuSVFfVE9UQUxfQ0wuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCJ3imrctYNkIJUNJUS4wLklRX1RPVEFMX0NMLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCNpXm7ctYNkIJUNJUS4wLklRX1RPVEFMX0NMLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCJ3imrctYNkIJENJUS4w</t>
+  </si>
+  <si>
+    <t>LklRX0xUX0RFQlQuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIyjCbty1g2QgkQ0lRLjAuSVFfTFRfREVCVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgLqpm3LWDZCCtDSVEuMC5JUV9MT05HX1RFUk1fTEVBU0VTLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhMH5q3LWDZCC1DSVEuMC5JUV9MT05HX1RFUk1fTEVBU0VTLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCG9tmrctYNkILUNJUS4wLklRX0xPTkdfVEVSTV9MRUFTRVMuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIneKaty1g2QgoQ0lRLjAuSVFfVU5FQVJOX1JFVl9MVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QgqQ0lRLjAuSVFfVU5FQVJOX1JFVl9MVC4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qid4pq3LWDZCCpDSVEuMC5J</t>
+  </si>
+  <si>
+    <t>UV9VTkVBUk5fUkVWX0xULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCNpXm7ctYNkIKkNJUS4wLklRX0RFRl9UQVhfTElBQl9MVC4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QgsQ0lRLjAuSVFfREVGX1RBWF9MSUFCX0xULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCAuqmbctYNkILENJUS4wLklRX0RFRl9UQVhfTElBQl9MVC4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qg5+Jm3LWDZCCVDSVEuMC5JUV9UT1RBTF9MSUFCLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhvbZq3LWDZCCdDSVEuMC5JUV9UT1RBTF9MSUFCLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCDn4mbctYNkIJ0NJUS4wLklRX1RPVEFMX0xJQUIuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QghQ0lRLjAuSVFf</t>
+  </si>
+  <si>
+    <t>Q09NTU9OLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qid4pq3LWDZCCNDSVEuMC5JUV9DT01NT04uLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI2lebty1g2QgjQ0lRLjAuSVFfQ09NTU9OLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCCfRmbctYNkIH0NJUS4wLklRX0FQSUMuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCACDmbctYNkIIUNJUS4wLklRX0FQSUMuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIOfiZty1g2QghQ0lRLjAuSVFfQVBJQy4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgAg5m3LWDZCB1DSVEuMC5JUV9SRS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIOfiZty1g2QgfQ0lRLjAuSVFfUkUuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBl</t>
+  </si>
+  <si>
+    <t>KczKebctYNkIb22aty1g2QgfQ0lRLjAuSVFfUkUuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIneKaty1g2QgjQ0lRLjAuSVFfVFJFQVNVUlkuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCNpXm7ctYNkIJUNJUS4wLklRX1RSRUFTVVJZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCMowm7ctYNkIJUNJUS4wLklRX1RSRUFTVVJZLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCACDmbctYNkIJ0NJUS4wLklRX09USEVSX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIswmbty1g2QgpQ0lRLjAuSVFfT1RIRVJfRVFVSVRZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCACDmbctYNkIKUNJUS4wLklRX09USEVSX0VRVUlUWS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qg5+Jm3LWDZCCZDSVEuMC5JUV9Q</t>
+  </si>
+  <si>
+    <t>UkVGX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QgoQ0lRLjAuSVFfUFJFRl9FUVVJVFkuLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIneKaty1g2QgoQ0lRLjAuSVFfUFJFRl9FUVVJVFkuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI2lebty1g2QgsQ0lRLjAuSVFfTUlOT1JJVFlfSU5URVJFU1QuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCPqlm7ctYNkILkNJUS4wLklRX01JTk9SSVRZX0lOVEVSRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCACDmbctYNkILkNJUS4wLklRX01JTk9SSVRZX0lOVEVSRVNULi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCDn4mbctYNkIJ0NJUS4wLklRX1RPVEFMX0VRVUlUWS4uMDA6MDA6MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QgpQ0lRLjAu</t>
+  </si>
+  <si>
+    <t>SVFfVE9UQUxfRVFVSVRZLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCHTXmrctYNkIKUNJUS4wLklRX1RPVEFMX0VRVUlUWS4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QjaV5u3LWDZCCRDSVEuMC5JUV9DQVNIX09QRVIuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCJK7mrctYNkIJkNJUS4wLklRX0NBU0hfT1BFUi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgAg5m3LWDZCCZDSVEuMC5JUV9DQVNIX09QRVIuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIOfiZty1g2QgmQ0lRLjAuSVFfQ0FTSF9JTlZFU1QuLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCG9tmrctYNkIKENJUS4wLklRX0NBU0hfSU5WRVNULi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCHTXmrctYNkIKENJUS4wLklRX0NBU0hfSU5WRVNULi4z</t>
+  </si>
+  <si>
+    <t>MS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCNpXm7ctYNkIJUNJUS4wLklRX0NBU0hfRklOQU4uLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCF1GmrctYNkIJ0NJUS4wLklRX0NBU0hfRklOQU4uLjMxLzEyLzE5MDAuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkI2lebty1g2QgnQ0lRLjAuSVFfQ0FTSF9GSU5BTi4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qj6pZu3LWDZCCVDSVEuMC5JUV9ORVRfQ0hBTkdFLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QgAg5m3LWDZCCdDSVEuMC5JUV9ORVRfQ0hBTkdFLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCDn4mbctYNkIJ0NJUS4wLklRX05FVF9DSEFOR0UuLjMxLzEyLzE5MDEuMC4wLjAuMAUAAAAAAAAACAAAABooSW52YWxpZCBSZXN0YXRlbWVudCBUeXBlKczKebctYNkIb22aty1g2QggQ0lRLjAuSVFfQ0FQRVguLjAwOjAwOjAwLjAuMC4wLjAFAAAAAAAAAAgA</t>
+  </si>
+  <si>
+    <t>AAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCHTXmrctYNkIIkNJUS4wLklRX0NBUEVYLi4zMS8xMi8xOTAwLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCNpXm7ctYNkIIkNJUS4wLklRX0NBUEVYLi4zMS8xMi8xOTAxLjAuMC4wLjAFAAAAAAAAAAgAAAAaKEludmFsaWQgUmVzdGF0ZW1lbnQgVHlwZSnMynm3LWDZCACDmbctYNkILENJUS4wLklRX1RPVEFMX0RJVl9QQUlEX0NGLi4wMDowMDowMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qg5+Jm3LWDZCC5DSVEuMC5JUV9UT1RBTF9ESVZfUEFJRF9DRi4uMzEvMTIvMTkwMC4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2QhvbZq3LWDZCC5DSVEuMC5JUV9UT1RBTF9ESVZfUEFJRF9DRi4uMzEvMTIvMTkwMS4wLjAuMC4wBQAAAAAAAAAIAAAAGihJbnZhbGlkIFJlc3RhdGVtZW50IFR5cGUpzMp5ty1g2Qh015q3LWDZCCJDSVEuMC5JUV9FQklUX0VTVC4uMDA6MDA6MDAuLjAuMC4wBQAAAAEAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKU2Y0bctYNkITZjRty1g2QgkQ0lRLjAuSVFfRUJJVERBX0VTVC4uMDA6MDA6MDAuLjAuMC4wBQAAAAEAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBN</t>
+  </si>
+  <si>
+    <t>b2RlKU2Y0bctYNkITZjRty1g2QggQ0lRLjAuSVFfREFfRVNULi4wMDowMDowMC4uMC4wLjAFAAAAAQAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpTZjRty1g2QhNmNG3LWDZCCVDSVEuMC5JUV9SRVZFTlVFX0VTVC4uMDA6MDA6MDAuLjAuMC4wBQAAAAEAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKU2Y0bctYNkITZjRty1g2QgqQ0lRLjAuSVFfR1JPU1NfTUFSR0lOX0VTVC4uMDA6MDA6MDAuLjAuMC4wBQAAAAEAAAAIAAAAFShJbnZhbGlkIEZpbGluZyBNb2RlKU2Y0bctYNkITZjRty1g2QgjQ0lRLjAuSVFfQ0FQRVhfRVNULi4wMDowMDowMC4uMC4wLjAFAAAAAQAAAAgAAAAVKEludmFsaWQgRmlsaW5nIE1vZGUpTZjRty1g2QhNmNG3LWDZCA==</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1492,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1568,6 +1550,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF1440AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1992,7 +1980,7 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="295">
+  <cellXfs count="298">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2351,9 +2339,6 @@
     <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="32" applyFont="1" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="9" borderId="0" xfId="26" applyFont="1" applyFill="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="169" fontId="10" fillId="9" borderId="0" xfId="18" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="10" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2452,7 +2437,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="45" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="18" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="10" fillId="0" borderId="9" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2562,29 +2546,40 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="10" fillId="11" borderId="0" xfId="18" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="8" fillId="11" borderId="0" xfId="26" applyFont="1" applyFill="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2674,42 +2669,42 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="FTI Theme">
   <a:themeElements>
-    <a:clrScheme name="FTI Colors">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="003763"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="003763"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="298DC1"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="D2CFCD"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="32006E"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="873299"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="FF661B"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="71B7E4"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -2989,351 +2984,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B017F0-02C3-43FE-8D0C-5E0F833F7572}">
-  <dimension ref="A1:H39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F410C3-B524-49FA-812E-5FA06FD17011}">
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="2.69140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="28.07421875" customWidth="1"/>
-    <col min="3" max="3" width="15.4609375" customWidth="1"/>
-    <col min="4" max="4" width="20.765625" customWidth="1"/>
-    <col min="5" max="6" width="13.07421875" customWidth="1"/>
-    <col min="7" max="8" width="15.84375" customWidth="1"/>
-    <col min="9" max="9" width="12.15234375" customWidth="1"/>
-    <col min="18" max="18" width="10.84375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
-      <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="242" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-    </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="229" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="72" t="s">
-        <v>262</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B10" s="72" t="s">
-        <v>232</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B11" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B12" s="72"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="163"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B13" s="229" t="s">
-        <v>275</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="163"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B14" s="72" t="s">
-        <v>277</v>
-      </c>
-      <c r="D14" s="108"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="72"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B15" s="72" t="s">
-        <v>274</v>
-      </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="72"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B16" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="72"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B17" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="72"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B19" s="229" t="s">
-        <v>276</v>
-      </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B20" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="234" t="s">
-        <v>203</v>
-      </c>
-      <c r="F20" s="234" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B21" s="72" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="163"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="72" t="s">
-        <v>263</v>
-      </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="163"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B23" s="72" t="s">
-        <v>233</v>
-      </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="222"/>
-      <c r="E23" s="163"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B25" s="229" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="163"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B26" s="72" t="s">
-        <v>264</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="223"/>
-      <c r="E26" s="111" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B27" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="223"/>
-      <c r="E27" s="163"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B28" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="223"/>
-      <c r="E28" s="163"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B29" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="223"/>
-      <c r="E29" s="163"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B30" s="72" t="s">
-        <v>261</v>
-      </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="223"/>
-      <c r="E30" s="163"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B31" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="222"/>
-      <c r="E31" s="163"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B32" s="72"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="163"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B33" s="229" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B34" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="108"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="78"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B35" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="234" t="s">
-        <v>33</v>
-      </c>
-      <c r="F35" s="234" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B36" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="107" t="s">
-        <v>281</v>
-      </c>
-      <c r="E36" s="113"/>
-      <c r="F36" s="72"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B37" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="72"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B38" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="113"/>
-      <c r="F38" s="72"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B39" s="72"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="163"/>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A1">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J1" t="s">
+        <v>304</v>
+      </c>
+      <c r="K1" t="s">
+        <v>305</v>
+      </c>
+      <c r="L1" t="s">
+        <v>306</v>
+      </c>
+      <c r="M1" t="s">
+        <v>307</v>
+      </c>
+      <c r="N1" t="s">
+        <v>308</v>
+      </c>
+      <c r="O1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P1" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>311</v>
+      </c>
+      <c r="R1" t="s">
+        <v>312</v>
+      </c>
+      <c r="S1" t="s">
+        <v>313</v>
+      </c>
+      <c r="T1" t="s">
+        <v>314</v>
+      </c>
+      <c r="U1" t="s">
+        <v>315</v>
+      </c>
+      <c r="V1" t="s">
+        <v>316</v>
+      </c>
+      <c r="W1" t="s">
+        <v>317</v>
+      </c>
+      <c r="X1" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>323</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16" xr:uid="{5406099E-438D-429E-94D2-B85C2A8D75D5}">
-      <formula1>"P,F"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20" xr:uid="{7B704DD2-4C7A-4F89-9DBF-0345CDF9086D}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17" xr:uid="{8FEECCD0-F4C3-4E9E-84F8-333E478DF84F}">
-      <formula1>"C, H"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35" xr:uid="{F46C7D24-8BA9-43BD-8E9A-45A4DCB7FF2D}">
-      <formula1>"Gross Debt, Net Debt"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3359,7 +3107,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3374,23 +3122,23 @@
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="G1" s="194"/>
+      <c r="G1" s="296"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -3399,21 +3147,21 @@
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="240" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="243"/>
-      <c r="J6" s="243"/>
-      <c r="K6" s="243"/>
-      <c r="L6" s="243"/>
-      <c r="M6" s="243"/>
-      <c r="N6" s="243"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="241"/>
+      <c r="I6" s="241"/>
+      <c r="J6" s="241"/>
+      <c r="K6" s="241"/>
+      <c r="L6" s="241"/>
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B8" s="116" t="s">
@@ -3428,7 +3176,7 @@
         <v>91</v>
       </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="228">
+      <c r="D9" s="227">
         <f>Assumptions!D9</f>
         <v>0</v>
       </c>
@@ -3439,7 +3187,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="50"/>
-      <c r="D10" s="228"/>
+      <c r="D10" s="227"/>
       <c r="E10" s="111" t="s">
         <v>36</v>
       </c>
@@ -3449,7 +3197,7 @@
         <v>196</v>
       </c>
       <c r="C11" s="50"/>
-      <c r="D11" s="230">
+      <c r="D11" s="229">
         <f>Assumptions!D14</f>
         <v>0</v>
       </c>
@@ -3460,7 +3208,7 @@
         <v>274</v>
       </c>
       <c r="C12" s="50"/>
-      <c r="D12" s="228">
+      <c r="D12" s="227">
         <f>Assumptions!D15</f>
         <v>0</v>
       </c>
@@ -3471,7 +3219,7 @@
         <v>38</v>
       </c>
       <c r="C13" s="50"/>
-      <c r="D13" s="228">
+      <c r="D13" s="227">
         <f>Assumptions!D16</f>
         <v>0</v>
       </c>
@@ -3480,7 +3228,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="D14" s="232"/>
+      <c r="D14" s="231"/>
       <c r="E14" s="115" t="s">
         <v>89</v>
       </c>
@@ -3490,7 +3238,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="228">
+      <c r="D15" s="227">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -3501,14 +3249,14 @@
         <v>16</v>
       </c>
       <c r="C16" s="50"/>
-      <c r="D16" s="228">
+      <c r="D16" s="227">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
       <c r="E16" s="110"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="D17" s="232"/>
+      <c r="D17" s="231"/>
       <c r="E17" s="114"/>
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -3979,7 +3727,7 @@
   <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3994,23 +3742,23 @@
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="G1" s="194"/>
+      <c r="G1" s="296"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4019,21 +3767,21 @@
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="240" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="243"/>
-      <c r="J6" s="243"/>
-      <c r="K6" s="243"/>
-      <c r="L6" s="243"/>
-      <c r="M6" s="243"/>
-      <c r="N6" s="243"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="241"/>
+      <c r="I6" s="241"/>
+      <c r="J6" s="241"/>
+      <c r="K6" s="241"/>
+      <c r="L6" s="241"/>
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B8" s="116" t="s">
@@ -4048,7 +3796,7 @@
         <v>91</v>
       </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="228">
+      <c r="D9" s="227">
         <f>Assumptions!D9</f>
         <v>0</v>
       </c>
@@ -4059,7 +3807,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="50"/>
-      <c r="D10" s="228"/>
+      <c r="D10" s="227"/>
       <c r="E10" s="111" t="s">
         <v>36</v>
       </c>
@@ -4069,7 +3817,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="50"/>
-      <c r="D11" s="230">
+      <c r="D11" s="229">
         <f>Assumptions!D14</f>
         <v>0</v>
       </c>
@@ -4080,7 +3828,7 @@
         <v>274</v>
       </c>
       <c r="C12" s="50"/>
-      <c r="D12" s="228">
+      <c r="D12" s="227">
         <f>Assumptions!D15</f>
         <v>0</v>
       </c>
@@ -4091,7 +3839,7 @@
         <v>38</v>
       </c>
       <c r="C13" s="50"/>
-      <c r="D13" s="228">
+      <c r="D13" s="227">
         <f>Assumptions!D16</f>
         <v>0</v>
       </c>
@@ -4100,7 +3848,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="D14" s="232"/>
+      <c r="D14" s="231"/>
       <c r="E14" s="115" t="s">
         <v>89</v>
       </c>
@@ -4110,7 +3858,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="228">
+      <c r="D15" s="227">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -4121,7 +3869,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="50"/>
-      <c r="D16" s="228">
+      <c r="D16" s="227">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
@@ -5080,10 +4828,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDC3174-2047-4F1B-B271-AD0AF164E1F3}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43:I44"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5098,23 +4846,23 @@
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="G1" s="194"/>
+      <c r="G1" s="296"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5123,21 +4871,21 @@
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="240" t="s">
         <v>205</v>
       </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="243"/>
-      <c r="J6" s="243"/>
-      <c r="K6" s="243"/>
-      <c r="L6" s="243"/>
-      <c r="M6" s="243"/>
-      <c r="N6" s="243"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="241"/>
+      <c r="I6" s="241"/>
+      <c r="J6" s="241"/>
+      <c r="K6" s="241"/>
+      <c r="L6" s="241"/>
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B8" s="116" t="s">
@@ -5152,7 +4900,7 @@
         <v>91</v>
       </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="228">
+      <c r="D9" s="227">
         <f>Assumptions!D9</f>
         <v>0</v>
       </c>
@@ -5163,7 +4911,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="50"/>
-      <c r="D10" s="228"/>
+      <c r="D10" s="227"/>
       <c r="E10" s="111" t="s">
         <v>36</v>
       </c>
@@ -5173,7 +4921,7 @@
         <v>196</v>
       </c>
       <c r="C11" s="50"/>
-      <c r="D11" s="230">
+      <c r="D11" s="229">
         <f>Assumptions!D14</f>
         <v>0</v>
       </c>
@@ -5184,7 +4932,7 @@
         <v>274</v>
       </c>
       <c r="C12" s="50"/>
-      <c r="D12" s="228">
+      <c r="D12" s="227">
         <f>Assumptions!D15</f>
         <v>0</v>
       </c>
@@ -5195,7 +4943,7 @@
         <v>38</v>
       </c>
       <c r="C13" s="50"/>
-      <c r="D13" s="228">
+      <c r="D13" s="227">
         <f>Assumptions!D16</f>
         <v>0</v>
       </c>
@@ -5204,7 +4952,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="D14" s="232"/>
+      <c r="D14" s="231"/>
       <c r="E14" s="115" t="s">
         <v>89</v>
       </c>
@@ -5214,7 +4962,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="228">
+      <c r="D15" s="227">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -5225,18 +4973,18 @@
         <v>16</v>
       </c>
       <c r="C16" s="50"/>
-      <c r="D16" s="228">
+      <c r="D16" s="227">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
       <c r="E16" s="110"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="D17" s="232"/>
+      <c r="D17" s="231"/>
       <c r="E17" s="114"/>
     </row>
     <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D18" s="232"/>
+      <c r="D18" s="231"/>
       <c r="K18" s="37"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.4">
@@ -5422,6 +5170,15 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.4">
+      <c r="I42" s="231"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.4">
+      <c r="I43" s="231"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.4">
+      <c r="I44" s="231"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5435,6 +5192,355 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B017F0-02C3-43FE-8D0C-5E0F833F7572}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="2.69140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="28.07421875" customWidth="1"/>
+    <col min="3" max="3" width="15.4609375" customWidth="1"/>
+    <col min="4" max="4" width="20.765625" customWidth="1"/>
+    <col min="5" max="6" width="13.07421875" customWidth="1"/>
+    <col min="7" max="8" width="15.84375" customWidth="1"/>
+    <col min="9" max="9" width="12.15234375" customWidth="1"/>
+    <col min="18" max="18" width="10.84375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
+      <c r="A2" s="8"/>
+      <c r="B2" s="253" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="8"/>
+      <c r="B3" s="239" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="8"/>
+      <c r="B4" s="239" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8"/>
+      <c r="B6" s="240" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+    </row>
+    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B8" s="228" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B9" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B10" s="72" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B11" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B12" s="72"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="163"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B13" s="228" t="s">
+        <v>275</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="163"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B14" s="72" t="s">
+        <v>277</v>
+      </c>
+      <c r="D14" s="108"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="72"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B15" s="72" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="72"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B16" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="50"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="72"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B17" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="50"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="72"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B19" s="228" t="s">
+        <v>276</v>
+      </c>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B20" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="233" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20" s="233" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B21" s="72" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="50"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="163"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B22" s="72" t="s">
+        <v>263</v>
+      </c>
+      <c r="C22" s="50"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="163"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B23" s="72" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="221"/>
+      <c r="E23" s="163"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B25" s="228" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="163"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B26" s="72" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="222"/>
+      <c r="E26" s="111" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B27" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="222"/>
+      <c r="E27" s="163"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B28" s="72" t="s">
+        <v>260</v>
+      </c>
+      <c r="C28" s="50"/>
+      <c r="D28" s="222"/>
+      <c r="E28" s="163"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B29" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="222"/>
+      <c r="E29" s="163"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B30" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="C30" s="50"/>
+      <c r="D30" s="222"/>
+      <c r="E30" s="163"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B31" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="50"/>
+      <c r="D31" s="221"/>
+      <c r="E31" s="163"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B32" s="72"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="163"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B33" s="228" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="50"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B34" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="50"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="78"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B35" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="50"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="233" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="233" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B36" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="50"/>
+      <c r="D36" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="E36" s="113"/>
+      <c r="F36" s="72"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B37" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="C37" s="50"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="72"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B38" s="72" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38" s="50"/>
+      <c r="D38" s="107"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="72"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B39" s="72"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="163"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16" xr:uid="{5406099E-438D-429E-94D2-B85C2A8D75D5}">
+      <formula1>"P,F"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20" xr:uid="{7B704DD2-4C7A-4F89-9DBF-0345CDF9086D}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17" xr:uid="{8FEECCD0-F4C3-4E9E-84F8-333E478DF84F}">
+      <formula1>"C, H"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35" xr:uid="{F46C7D24-8BA9-43BD-8E9A-45A4DCB7FF2D}">
+      <formula1>"Gross Debt, Net Debt"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3A03BB-2253-4F2B-9E20-F3B7AE788215}">
   <sheetPr>
     <tabColor rgb="FF1440AA"/>
@@ -5451,12 +5557,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74EC6BE-E931-459B-9911-101FA66B3EAA}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5474,19 +5580,19 @@
     </row>
     <row r="2" spans="1:9" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5498,10 +5604,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
-      <c r="B6" s="244" t="s">
+      <c r="B6" s="242" t="s">
         <v>229</v>
       </c>
-      <c r="C6" s="245"/>
+      <c r="C6" s="243"/>
       <c r="E6" s="21"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -5515,10 +5621,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="8"/>
-      <c r="B8" s="246" t="s">
+      <c r="B8" s="244" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="247">
+      <c r="C8" s="245">
         <f>Assumptions!$D$10</f>
         <v>0</v>
       </c>
@@ -5527,30 +5633,30 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B9" s="248" t="s">
+      <c r="B9" s="246" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="249">
+      <c r="C9" s="247">
         <f>Assumptions!$D$23</f>
         <v>0</v>
       </c>
       <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B10" s="248" t="s">
+      <c r="B10" s="246" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="249">
+      <c r="C10" s="247">
         <f>Assumptions!$D$31</f>
         <v>0</v>
       </c>
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="250" t="s">
+      <c r="B11" s="248" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="251" t="e">
+      <c r="C11" s="249" t="e">
         <f>IF(OR(ISBLANK(Assumptions!D26),Assumptions!D26=""),'Discount rate'!C26,Assumptions!D26)</f>
         <v>#VALUE!</v>
       </c>
@@ -5637,16 +5743,16 @@
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B23" s="244" t="s">
+      <c r="B23" s="242" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="244"/>
-      <c r="D23" s="244"/>
-      <c r="E23" s="244"/>
-      <c r="F23" s="244"/>
-      <c r="G23" s="244"/>
-      <c r="H23" s="244"/>
-      <c r="I23" s="244"/>
+      <c r="C23" s="242"/>
+      <c r="D23" s="242"/>
+      <c r="E23" s="242"/>
+      <c r="F23" s="242"/>
+      <c r="G23" s="242"/>
+      <c r="H23" s="242"/>
+      <c r="I23" s="242"/>
       <c r="J23" s="7" t="s">
         <v>278</v>
       </c>
@@ -5661,7 +5767,7 @@
         <f>DATE(YEAR($F$24)+COLUMN(E24)-COLUMN($F$24),MONTH($F$24),DAY($F$24))</f>
         <v>693597</v>
       </c>
-      <c r="F24" s="235">
+      <c r="F24" s="295">
         <f>forecastStart</f>
         <v>0</v>
       </c>
@@ -5773,15 +5879,15 @@
       <c r="C28" s="171" t="s">
         <v>218</v>
       </c>
-      <c r="F28" s="236" t="e">
+      <c r="F28" s="234" t="e">
         <f ca="1">F27/OFFSET(F27,0,-1)-1</f>
         <v>#N/A</v>
       </c>
-      <c r="G28" s="236" t="e">
+      <c r="G28" s="234" t="e">
         <f t="shared" ref="G28:H28" ca="1" si="2">G27/OFFSET(G27,0,-1)-1</f>
         <v>#N/A</v>
       </c>
-      <c r="H28" s="236" t="e">
+      <c r="H28" s="234" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#N/A</v>
       </c>
@@ -5818,30 +5924,30 @@
         <f>INDEX(Forecasts!$14:$14,MATCH(H$25,Forecasts!$11:$11,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="I29" s="263"/>
+      <c r="I29" s="261"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B30" s="30"/>
       <c r="C30" s="171" t="s">
         <v>287</v>
       </c>
-      <c r="D30" s="236" t="e">
+      <c r="D30" s="234" t="e">
         <f>D31/D27</f>
         <v>#N/A</v>
       </c>
-      <c r="E30" s="236" t="e">
+      <c r="E30" s="234" t="e">
         <f t="shared" ref="E30:H30" si="3">E31/E27</f>
         <v>#N/A</v>
       </c>
-      <c r="F30" s="236" t="e">
+      <c r="F30" s="234" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="G30" s="236" t="e">
+      <c r="G30" s="234" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="H30" s="236" t="e">
+      <c r="H30" s="234" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
@@ -5851,28 +5957,28 @@
       <c r="B31" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="264"/>
-      <c r="D31" s="265" t="e">
+      <c r="C31" s="262"/>
+      <c r="D31" s="263" t="e">
         <f>D27+D29</f>
         <v>#N/A</v>
       </c>
-      <c r="E31" s="265" t="e">
+      <c r="E31" s="263" t="e">
         <f>E27+E29</f>
         <v>#N/A</v>
       </c>
-      <c r="F31" s="265" t="e">
+      <c r="F31" s="263" t="e">
         <f>F27+F29</f>
         <v>#N/A</v>
       </c>
-      <c r="G31" s="265" t="e">
+      <c r="G31" s="263" t="e">
         <f>G27+G29</f>
         <v>#N/A</v>
       </c>
-      <c r="H31" s="265" t="e">
+      <c r="H31" s="263" t="e">
         <f>H27+H29</f>
         <v>#N/A</v>
       </c>
-      <c r="I31" s="265"/>
+      <c r="I31" s="263"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B32" s="7" t="s">
@@ -5910,15 +6016,15 @@
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="236" t="e">
+      <c r="F33" s="234" t="e">
         <f>F34/F27</f>
         <v>#N/A</v>
       </c>
-      <c r="G33" s="236" t="e">
+      <c r="G33" s="234" t="e">
         <f>G34/G27</f>
         <v>#N/A</v>
       </c>
-      <c r="H33" s="236" t="e">
+      <c r="H33" s="234" t="e">
         <f>H34/H27</f>
         <v>#N/A</v>
       </c>
@@ -5959,19 +6065,19 @@
         <v>55</v>
       </c>
       <c r="D35" s="10"/>
-      <c r="E35" s="237">
+      <c r="E35" s="235">
         <f>$C$10</f>
         <v>0</v>
       </c>
-      <c r="F35" s="237">
+      <c r="F35" s="235">
         <f t="shared" ref="F35:H35" si="4">$C$10</f>
         <v>0</v>
       </c>
-      <c r="G35" s="237">
+      <c r="G35" s="235">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H35" s="237">
+      <c r="H35" s="235">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6112,23 +6218,23 @@
         <v>224</v>
       </c>
       <c r="C41" s="131"/>
-      <c r="D41" s="238" t="e">
+      <c r="D41" s="236" t="e">
         <f>SUM(D42:D43)</f>
         <v>#N/A</v>
       </c>
-      <c r="E41" s="238" t="e">
+      <c r="E41" s="236" t="e">
         <f>SUM(E42:E43)</f>
         <v>#N/A</v>
       </c>
-      <c r="F41" s="238" t="e">
+      <c r="F41" s="236" t="e">
         <f ca="1">OFFSET(F41,0,-1)-F39</f>
         <v>#N/A</v>
       </c>
-      <c r="G41" s="238" t="e">
+      <c r="G41" s="236" t="e">
         <f t="shared" ref="G41:H41" ca="1" si="6">OFFSET(G41,0,-1)-G39</f>
         <v>#N/A</v>
       </c>
-      <c r="H41" s="238" t="e">
+      <c r="H41" s="236" t="e">
         <f t="shared" ca="1" si="6"/>
         <v>#N/A</v>
       </c>
@@ -6185,19 +6291,19 @@
         <v>219</v>
       </c>
       <c r="D44" s="34"/>
-      <c r="E44" s="239" t="e">
+      <c r="E44" s="237" t="e">
         <f>IF(E41/E27&lt;0, "n/a", E41/E27)</f>
         <v>#N/A</v>
       </c>
-      <c r="F44" s="239" t="e">
+      <c r="F44" s="237" t="e">
         <f ca="1">IF(F41/F27&lt;0, "NM", F41/F27)</f>
         <v>#N/A</v>
       </c>
-      <c r="G44" s="239" t="e">
+      <c r="G44" s="237" t="e">
         <f ca="1">IF(G41/G27&lt;0, "NM", G41/G27)</f>
         <v>#N/A</v>
       </c>
-      <c r="H44" s="239" t="e">
+      <c r="H44" s="237" t="e">
         <f ca="1">IF(H41/H27&lt;0, "NM", H41/H27)</f>
         <v>#N/A</v>
       </c>
@@ -6343,15 +6449,15 @@
       <c r="C50" s="171" t="s">
         <v>220</v>
       </c>
-      <c r="F50" s="240" t="e">
+      <c r="F50" s="238" t="e">
         <f t="shared" ref="F50:H50" ca="1" si="10">F49/OFFSET(F49,0,-1)-1</f>
         <v>#N/A</v>
       </c>
-      <c r="G50" s="240" t="e">
+      <c r="G50" s="238" t="e">
         <f t="shared" ca="1" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="H50" s="240" t="e">
+      <c r="H50" s="238" t="e">
         <f t="shared" ca="1" si="10"/>
         <v>#N/A</v>
       </c>
@@ -6419,7 +6525,7 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
-      <c r="G53" s="194"/>
+      <c r="G53" s="296"/>
       <c r="H53" s="10"/>
     </row>
   </sheetData>
@@ -6429,7 +6535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C95108-EDE0-4179-8B50-FB6BC550E7AC}">
   <sheetPr>
     <tabColor rgb="FF1440AA"/>
@@ -6446,7 +6552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372557FB-CD81-4240-B67F-6856EAF8E929}">
   <dimension ref="A1:T27"/>
   <sheetViews>
@@ -6472,19 +6578,19 @@
     </row>
     <row r="2" spans="1:20" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -6493,10 +6599,10 @@
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="B6" s="244" t="s">
+      <c r="B6" s="242" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="252"/>
+      <c r="C6" s="250"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -6529,7 +6635,7 @@
       <c r="B8" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="195">
+      <c r="C8" s="194">
         <f>Assumptions!D27</f>
         <v>0</v>
       </c>
@@ -6551,7 +6657,7 @@
       <c r="B9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="224" t="e">
+      <c r="C9" s="223" t="e">
         <f>Beta!$D$12</f>
         <v>#VALUE!</v>
       </c>
@@ -6573,7 +6679,7 @@
       <c r="B10" s="25" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="225">
+      <c r="C10" s="224">
         <f>Assumptions!D28</f>
         <v>0</v>
       </c>
@@ -6592,7 +6698,7 @@
       <c r="T10" s="12"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="C11" s="226"/>
+      <c r="C11" s="225"/>
       <c r="E11" s="30"/>
       <c r="I11" s="12"/>
       <c r="J11" s="40"/>
@@ -6611,7 +6717,7 @@
       <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="227" t="e">
+      <c r="C12" s="226" t="e">
         <f>C8+(C9*C10)</f>
         <v>#VALUE!</v>
       </c>
@@ -6630,7 +6736,7 @@
       <c r="T12" s="12"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="C13" s="226"/>
+      <c r="C13" s="225"/>
       <c r="E13" s="30"/>
       <c r="I13" s="12"/>
       <c r="J13" s="40"/>
@@ -6649,7 +6755,7 @@
       <c r="B14" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="C14" s="195">
+      <c r="C14" s="194">
         <f>Assumptions!D29</f>
         <v>0</v>
       </c>
@@ -6671,7 +6777,7 @@
       <c r="B15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="225">
+      <c r="C15" s="224">
         <f>DCF!$C$10</f>
         <v>0</v>
       </c>
@@ -6690,7 +6796,7 @@
       <c r="T15" s="12"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="C16" s="226"/>
+      <c r="C16" s="225"/>
       <c r="E16" s="30"/>
       <c r="I16" s="12"/>
       <c r="J16" s="40"/>
@@ -6709,7 +6815,7 @@
       <c r="B17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="227">
+      <c r="C17" s="226">
         <f>C14*(1-C15)</f>
         <v>0</v>
       </c>
@@ -6728,7 +6834,7 @@
       <c r="T17" s="12"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="C18" s="226"/>
+      <c r="C18" s="225"/>
       <c r="E18" s="30"/>
       <c r="I18" s="12"/>
       <c r="J18" s="40"/>
@@ -6747,7 +6853,7 @@
       <c r="B19" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="195">
+      <c r="C19" s="194">
         <f>1-C22</f>
         <v>1</v>
       </c>
@@ -6900,15 +7006,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B36D92-2F89-45DC-B207-E3875F4AA818}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6946,19 +7052,19 @@
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -6967,11 +7073,11 @@
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="60" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="253" t="s">
+      <c r="B6" s="251" t="s">
         <v>246</v>
       </c>
-      <c r="C6" s="253"/>
-      <c r="D6" s="254"/>
+      <c r="C6" s="251"/>
+      <c r="D6" s="252"/>
       <c r="E6" s="7"/>
       <c r="F6" s="189" t="s">
         <v>247</v>
@@ -7102,25 +7208,25 @@
       <c r="I15" s="7"/>
     </row>
     <row r="17" spans="2:18" s="60" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="253" t="s">
+      <c r="B17" s="251" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="253"/>
-      <c r="D17" s="254"/>
-      <c r="E17" s="254"/>
-      <c r="F17" s="254"/>
-      <c r="G17" s="254"/>
-      <c r="H17" s="254"/>
-      <c r="I17" s="254"/>
-      <c r="J17" s="254"/>
-      <c r="K17" s="254"/>
-      <c r="L17" s="254"/>
-      <c r="M17" s="254"/>
-      <c r="N17" s="254"/>
-      <c r="O17" s="254"/>
-      <c r="P17" s="254"/>
-      <c r="Q17" s="254"/>
-      <c r="R17" s="254"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="252"/>
+      <c r="E17" s="252"/>
+      <c r="F17" s="252"/>
+      <c r="G17" s="252"/>
+      <c r="H17" s="252"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="252"/>
+      <c r="K17" s="252"/>
+      <c r="L17" s="252"/>
+      <c r="M17" s="252"/>
+      <c r="N17" s="252"/>
+      <c r="O17" s="252"/>
+      <c r="P17" s="252"/>
+      <c r="Q17" s="252"/>
+      <c r="R17" s="252"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B19" s="97" t="s">
@@ -7152,7 +7258,7 @@
       <c r="B21" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="228">
+      <c r="D21" s="227">
         <f>Assumptions!D35</f>
         <v>0</v>
       </c>
@@ -7217,7 +7323,7 @@
       <c r="B24" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="228"/>
+      <c r="D24" s="227"/>
       <c r="E24" s="79" t="s">
         <v>36</v>
       </c>
@@ -7239,7 +7345,7 @@
       <c r="B25" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="230">
+      <c r="D25" s="229">
         <f>Assumptions!D34</f>
         <v>0</v>
       </c>
@@ -7262,7 +7368,7 @@
       <c r="B26" s="72" t="s">
         <v>274</v>
       </c>
-      <c r="D26" s="228">
+      <c r="D26" s="227">
         <f>Assumptions!D15</f>
         <v>0</v>
       </c>
@@ -7285,7 +7391,7 @@
       <c r="B27" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="228">
+      <c r="D27" s="227">
         <f>Assumptions!D16</f>
         <v>0</v>
       </c>
@@ -7310,7 +7416,7 @@
       <c r="B28" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="228">
+      <c r="D28" s="227">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -7333,7 +7439,7 @@
       <c r="B29" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="228">
+      <c r="D29" s="227">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
@@ -7394,7 +7500,7 @@
       <c r="B32" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="230">
+      <c r="D32" s="229">
         <f>Assumptions!D34</f>
         <v>0</v>
       </c>
@@ -7417,7 +7523,7 @@
       <c r="B33" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="230">
+      <c r="D33" s="229">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -7440,7 +7546,7 @@
       <c r="B34" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="230">
+      <c r="D34" s="229">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
@@ -7501,7 +7607,7 @@
       <c r="B37" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="230">
+      <c r="D37" s="229">
         <f>DATE(YEAR(D38)-2,MONTH(D38),DAY(D38))</f>
         <v>693232</v>
       </c>
@@ -7524,7 +7630,7 @@
       <c r="B38" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="230">
+      <c r="D38" s="229">
         <f>D25</f>
         <v>0</v>
       </c>
@@ -7547,7 +7653,7 @@
       <c r="B39" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="228" t="str">
+      <c r="D39" s="227" t="str">
         <f>Assumptions!D36</f>
         <v>W</v>
       </c>
@@ -7570,7 +7676,7 @@
       <c r="B40" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="228">
+      <c r="D40" s="227">
         <f>Assumptions!D38</f>
         <v>0</v>
       </c>
@@ -7595,7 +7701,7 @@
       <c r="B41" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="231">
+      <c r="D41" s="230">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -7618,7 +7724,7 @@
       <c r="B42" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="231">
+      <c r="D42" s="230">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
@@ -7633,10 +7739,10 @@
       <c r="M42" s="72"/>
       <c r="N42" s="72"/>
       <c r="O42" s="189" t="s">
-        <v>329</v>
-      </c>
-      <c r="P42" s="262"/>
-      <c r="Q42" s="262"/>
+        <v>295</v>
+      </c>
+      <c r="P42" s="260"/>
+      <c r="Q42" s="260"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B43" s="72"/>
@@ -7677,16 +7783,16 @@
       <c r="R44" s="72"/>
     </row>
     <row r="45" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="B45" s="196" t="s">
+      <c r="B45" s="195" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="196" t="s">
+      <c r="C45" s="195" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="196" t="s">
+      <c r="D45" s="195" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="196"/>
+      <c r="E45" s="195"/>
       <c r="F45" s="94" t="s">
         <v>47</v>
       </c>
@@ -7799,46 +7905,46 @@
       <c r="R47" s="72"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A48" s="193"/>
-      <c r="B48" s="257" t="str" cm="1">
+      <c r="A48" s="297"/>
+      <c r="B48" s="255" t="str" cm="1">
         <f t="array" ref="B48">_xll.ciqfunctions.udf.CIQ($C48,B$46)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="C48" s="258"/>
-      <c r="D48" s="259" t="str" cm="1">
+      <c r="C48" s="256"/>
+      <c r="D48" s="257" t="str" cm="1">
         <f t="array" ref="D48">_xll.ciqfunctions.udf.CIQ($C48,D$46,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="E48" s="259"/>
-      <c r="F48" s="259" t="str" cm="1">
+      <c r="E48" s="257"/>
+      <c r="F48" s="257" t="str" cm="1">
         <f t="array" ref="F48">_xll.ciqfunctions.udf.CIQ($C48,F$46,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="G48" s="259" t="str" cm="1">
+      <c r="G48" s="257" t="str" cm="1">
         <f t="array" ref="G48">_xll.ciqfunctions.udf.CIQ($C48,G$46,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="H48" s="259" t="str" cm="1">
+      <c r="H48" s="257" t="str" cm="1">
         <f t="array" ref="H48">_xll.ciqfunctions.udf.CIQ($C48,H$46,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="I48" s="260">
+      <c r="I48" s="258">
         <f t="shared" ref="I48" si="0">SUM(G48:H48)</f>
         <v>0</v>
       </c>
-      <c r="J48" s="259" t="str" cm="1">
+      <c r="J48" s="257" t="str" cm="1">
         <f t="array" ref="J48">_xll.ciqfunctions.udf.CIQ($C48,J$46,$D$32,$D$33,$D$34)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="K48" s="256" t="str" cm="1">
+      <c r="K48" s="254" t="str" cm="1">
         <f t="array" ref="K48">_xll.ciqfunctions.udf.CIQ($C48,K$46,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="L48" s="256" t="str" cm="1">
+      <c r="L48" s="254" t="str" cm="1">
         <f t="array" ref="L48">_xll.ciqfunctions.udf.CIQAVG($C48,L$46,$D$37,$D$38)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="M48" s="260" t="str" cm="1">
+      <c r="M48" s="258" t="str" cm="1">
         <f t="array" ref="M48">_xll.ciqfunctions.udf.CIQ($C48,M$46,$D$37,$D$38,$D$39,$D$40,$D$41,$D$42)</f>
         <v>(Invalid Identifier)</v>
       </c>
@@ -7850,7 +7956,7 @@
         <f>MAX(I48/SUM(J48),0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P48" s="261">
+      <c r="P48" s="259">
         <v>0.25</v>
       </c>
       <c r="Q48" s="103" t="e">
@@ -7860,22 +7966,22 @@
       <c r="R48" s="72"/>
     </row>
     <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="193"/>
-      <c r="B49" s="257"/>
-      <c r="C49" s="258"/>
-      <c r="D49" s="259"/>
-      <c r="E49" s="259"/>
-      <c r="F49" s="259"/>
-      <c r="G49" s="259"/>
-      <c r="H49" s="259"/>
-      <c r="I49" s="260"/>
-      <c r="J49" s="259"/>
-      <c r="K49" s="256"/>
-      <c r="L49" s="256"/>
-      <c r="M49" s="260"/>
+      <c r="A49" s="297"/>
+      <c r="B49" s="255"/>
+      <c r="C49" s="256"/>
+      <c r="D49" s="257"/>
+      <c r="E49" s="257"/>
+      <c r="F49" s="257"/>
+      <c r="G49" s="257"/>
+      <c r="H49" s="257"/>
+      <c r="I49" s="258"/>
+      <c r="J49" s="257"/>
+      <c r="K49" s="254"/>
+      <c r="L49" s="254"/>
+      <c r="M49" s="258"/>
       <c r="N49" s="101"/>
       <c r="O49" s="102"/>
-      <c r="P49" s="261"/>
+      <c r="P49" s="259"/>
       <c r="Q49" s="103"/>
       <c r="R49" s="72"/>
     </row>
@@ -8036,12 +8142,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB39DFEB-ADE6-4ED5-9A3D-E259DD219367}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8062,19 +8168,19 @@
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
       <c r="I4"/>
@@ -8086,15 +8192,15 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="240" t="s">
         <v>229</v>
       </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="243"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="241"/>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -8115,7 +8221,7 @@
         <v>232</v>
       </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="230">
+      <c r="D9" s="229">
         <f>Assumptions!D10</f>
         <v>0</v>
       </c>
@@ -8126,7 +8232,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="50"/>
-      <c r="D10" s="228" t="s">
+      <c r="D10" s="227" t="s">
         <v>249</v>
       </c>
       <c r="E10" s="111"/>
@@ -8134,7 +8240,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B11" s="72"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="220"/>
+      <c r="D11" s="219"/>
       <c r="E11" s="111"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -8142,7 +8248,7 @@
         <v>91</v>
       </c>
       <c r="C12" s="50"/>
-      <c r="D12" s="228">
+      <c r="D12" s="227">
         <f>Assumptions!D9</f>
         <v>0</v>
       </c>
@@ -8153,7 +8259,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="50"/>
-      <c r="D13" s="228"/>
+      <c r="D13" s="227"/>
       <c r="E13" s="111" t="s">
         <v>36</v>
       </c>
@@ -8163,7 +8269,7 @@
         <v>274</v>
       </c>
       <c r="C14" s="50"/>
-      <c r="D14" s="228">
+      <c r="D14" s="227">
         <f>Assumptions!D15</f>
         <v>0</v>
       </c>
@@ -8174,7 +8280,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="228">
+      <c r="D15" s="227">
         <f>Assumptions!D16</f>
         <v>0</v>
       </c>
@@ -8183,7 +8289,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D16" s="232"/>
+      <c r="D16" s="231"/>
       <c r="E16" s="115" t="s">
         <v>89</v>
       </c>
@@ -8193,7 +8299,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="50"/>
-      <c r="D17" s="228">
+      <c r="D17" s="227">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
@@ -8204,7 +8310,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="50"/>
-      <c r="D18" s="228">
+      <c r="D18" s="227">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
@@ -8221,20 +8327,20 @@
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="8"/>
-      <c r="B21" s="212"/>
-      <c r="C21" s="208"/>
-      <c r="D21" s="209" t="s">
+      <c r="B21" s="211"/>
+      <c r="C21" s="207"/>
+      <c r="D21" s="208" t="s">
         <v>12</v>
       </c>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="8"/>
-      <c r="B22" s="215" t="s">
+      <c r="B22" s="214" t="s">
         <v>250</v>
       </c>
-      <c r="C22" s="208"/>
-      <c r="D22" s="214" t="e">
+      <c r="C22" s="207"/>
+      <c r="D22" s="213" t="e">
         <f>D40</f>
         <v>#NUM!</v>
       </c>
@@ -8242,11 +8348,11 @@
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="8"/>
-      <c r="B23" s="216" t="s">
+      <c r="B23" s="215" t="s">
         <v>255</v>
       </c>
       <c r="C23" s="88"/>
-      <c r="D23" s="210" t="str">
+      <c r="D23" s="209" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$12, "IQ_EBITDA", $D$10, $D$9, $D$14, $D$15, $D$17, $D$17)</f>
         <v>(Invalid Restatement Type)</v>
       </c>
@@ -8254,11 +8360,11 @@
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="8"/>
-      <c r="B24" s="217" t="s">
+      <c r="B24" s="216" t="s">
         <v>256</v>
       </c>
       <c r="C24" s="43"/>
-      <c r="D24" s="218" t="e">
+      <c r="D24" s="217" t="e">
         <f>D22*D23</f>
         <v>#NUM!</v>
       </c>
@@ -8266,11 +8372,11 @@
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="8"/>
-      <c r="B25" s="216" t="s">
+      <c r="B25" s="215" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="88"/>
-      <c r="D25" s="210" t="e" cm="1">
+      <c r="D25" s="209" t="e" cm="1">
         <f t="array" ref="D25">-_xll.ciqfunctions.udf.CIQ($D$12,"IQ_ST_DEBT",$D$13,$D$9,$D$14,$D$15,$D$17,$D$18)-_xll.ciqfunctions.udf.CIQ($D$12,"IQ_LT_DEBT",$D$13,$D$9,$D$14,$D$15,$D$17,$D$18)</f>
         <v>#VALUE!</v>
       </c>
@@ -8278,11 +8384,11 @@
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="8"/>
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="218" t="s">
         <v>71</v>
       </c>
       <c r="C26" s="89"/>
-      <c r="D26" s="211" t="str" cm="1">
+      <c r="D26" s="210" t="str" cm="1">
         <f t="array" ref="D26">_xll.ciqfunctions.udf.CIQ($D$12,"IQ_CASH_EQUIV",$D$13,$D$9,$D$14,$D$15,$D$17,$D$18)</f>
         <v>(Invalid Restatement Type)</v>
       </c>
@@ -8290,11 +8396,11 @@
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="8"/>
-      <c r="B27" s="213" t="s">
+      <c r="B27" s="212" t="s">
         <v>257</v>
       </c>
       <c r="C27" s="19"/>
-      <c r="D27" s="221" t="e">
+      <c r="D27" s="220" t="e">
         <f>SUM(D24:D26)</f>
         <v>#NUM!</v>
       </c>
@@ -8312,15 +8418,15 @@
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="8"/>
-      <c r="B30" s="242" t="s">
+      <c r="B30" s="240" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="243"/>
-      <c r="D30" s="243"/>
-      <c r="E30" s="243"/>
-      <c r="F30" s="243"/>
-      <c r="G30" s="243"/>
-      <c r="H30" s="243"/>
+      <c r="C30" s="241"/>
+      <c r="D30" s="241"/>
+      <c r="E30" s="241"/>
+      <c r="F30" s="241"/>
+      <c r="G30" s="241"/>
+      <c r="H30" s="241"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -8338,10 +8444,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B33" s="196" t="s">
+      <c r="B33" s="195" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="196" t="s">
+      <c r="C33" s="195" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="94" t="s">
@@ -8383,98 +8489,98 @@
       <c r="H35" s="83"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A36" s="194"/>
+      <c r="A36" s="296"/>
       <c r="B36" s="191" t="str" cm="1">
         <f t="array" ref="B36">_xll.ciqfunctions.udf.CIQ($C36,$B$34)</f>
         <v>(Invalid Identifier)</v>
       </c>
       <c r="C36" s="192"/>
-      <c r="D36" s="197" t="str">
+      <c r="D36" s="196" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($C36, D$34, $D$10, $D$9)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="F36" s="203" t="str">
+      <c r="F36" s="202" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($C36, F$34, $D$10, $D$9)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="G36" s="203" t="str">
+      <c r="G36" s="202" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($C36, G$34, $D$10, $D$9)</f>
         <v>(Invalid Identifier)</v>
       </c>
-      <c r="H36" s="204" t="str">
+      <c r="H36" s="203" t="str">
         <f>IFERROR(F36/G36,"NM")</f>
         <v>NM</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="194"/>
+      <c r="A37" s="296"/>
       <c r="B37" s="191"/>
       <c r="C37" s="192"/>
-      <c r="D37" s="197"/>
-      <c r="F37" s="203"/>
-      <c r="G37" s="203"/>
-      <c r="H37" s="204"/>
+      <c r="D37" s="196"/>
+      <c r="F37" s="202"/>
+      <c r="G37" s="202"/>
+      <c r="H37" s="203"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B38" s="119" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="119"/>
-      <c r="D38" s="200">
+      <c r="D38" s="199">
         <f>MIN($D$36:D37)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="200"/>
-      <c r="G38" s="200"/>
-      <c r="H38" s="205">
+      <c r="F38" s="199"/>
+      <c r="G38" s="199"/>
+      <c r="H38" s="204">
         <f>MIN($H$36:H37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B39" s="198" t="s">
+      <c r="B39" s="197" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="198"/>
-      <c r="D39" s="201">
+      <c r="C39" s="197"/>
+      <c r="D39" s="200">
         <f>MAX($D$36:D37)</f>
         <v>0</v>
       </c>
-      <c r="F39" s="201"/>
-      <c r="G39" s="201"/>
-      <c r="H39" s="206">
+      <c r="F39" s="200"/>
+      <c r="G39" s="200"/>
+      <c r="H39" s="205">
         <f>MAX($H$36:H37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B40" s="198" t="s">
+      <c r="B40" s="197" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="198"/>
-      <c r="D40" s="201" t="e">
+      <c r="C40" s="197"/>
+      <c r="D40" s="200" t="e">
         <f>MEDIAN($D$36:D37)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F40" s="201"/>
-      <c r="G40" s="201"/>
-      <c r="H40" s="206" t="e">
+      <c r="F40" s="200"/>
+      <c r="G40" s="200"/>
+      <c r="H40" s="205" t="e">
         <f>MEDIAN($H$36:H37)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="199" t="s">
+      <c r="B41" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="199"/>
-      <c r="D41" s="202" t="e">
+      <c r="C41" s="198"/>
+      <c r="D41" s="201" t="e">
         <f>AVERAGE($D$36:D37)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F41" s="202"/>
-      <c r="G41" s="202"/>
-      <c r="H41" s="207" t="e">
+      <c r="F41" s="201"/>
+      <c r="G41" s="201"/>
+      <c r="H41" s="206" t="e">
         <f>AVERAGE($H$36:H37)</f>
         <v>#DIV/0!</v>
       </c>
@@ -8495,132 +8601,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D09C6E1-6D41-4A30-B58A-D6A78E74C0B5}">
-  <dimension ref="A1:AI1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
-      <c r="A1">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G1" t="s">
-        <v>300</v>
-      </c>
-      <c r="H1" t="s">
-        <v>301</v>
-      </c>
-      <c r="I1" t="s">
-        <v>302</v>
-      </c>
-      <c r="J1" t="s">
-        <v>303</v>
-      </c>
-      <c r="K1" t="s">
-        <v>304</v>
-      </c>
-      <c r="L1" t="s">
-        <v>305</v>
-      </c>
-      <c r="M1" t="s">
-        <v>306</v>
-      </c>
-      <c r="N1" t="s">
-        <v>307</v>
-      </c>
-      <c r="O1" t="s">
-        <v>308</v>
-      </c>
-      <c r="P1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>310</v>
-      </c>
-      <c r="R1" t="s">
-        <v>311</v>
-      </c>
-      <c r="S1" t="s">
-        <v>312</v>
-      </c>
-      <c r="T1" t="s">
-        <v>313</v>
-      </c>
-      <c r="U1" t="s">
-        <v>314</v>
-      </c>
-      <c r="V1" t="s">
-        <v>315</v>
-      </c>
-      <c r="W1" t="s">
-        <v>316</v>
-      </c>
-      <c r="X1" t="s">
-        <v>317</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>318</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>319</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>320</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>321</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>322</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>323</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>324</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>326</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>327</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F336EB3-AE15-435C-BFD5-7698A0145ECB}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8636,23 +8622,23 @@
     <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="G1" s="194"/>
+      <c r="G1" s="193"/>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="16.75" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="253" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="239" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="239" t="s">
         <v>269</v>
       </c>
     </row>
@@ -8662,14 +8648,14 @@
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="240" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="243"/>
-      <c r="D6" s="243"/>
-      <c r="E6" s="243"/>
-      <c r="F6" s="243"/>
-      <c r="G6" s="243"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
     </row>
     <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8"/>
@@ -8680,7 +8666,7 @@
       <c r="B8" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D8" s="228">
+      <c r="D8" s="227">
         <f>Assumptions!D20</f>
         <v>0</v>
       </c>
@@ -8750,15 +8736,15 @@
       </c>
       <c r="C13"/>
       <c r="D13" s="130"/>
-      <c r="E13" s="266" t="e">
+      <c r="E13" s="264" t="e">
         <f>IF($D$8=$E$8,IF(NOT(E40=0),E40,E56),E56)</f>
         <v>#N/A</v>
       </c>
-      <c r="F13" s="266" t="e">
+      <c r="F13" s="264" t="e">
         <f>IF($D$8=$E$8,IF(NOT(F40=0),F40,F56),F56)</f>
         <v>#N/A</v>
       </c>
-      <c r="G13" s="266" t="e">
+      <c r="G13" s="264" t="e">
         <f>IF($D$8=$E$8,IF(NOT(G40=0),G40,G56),G56)</f>
         <v>#N/A</v>
       </c>
@@ -8770,15 +8756,15 @@
       </c>
       <c r="C14"/>
       <c r="D14" s="130"/>
-      <c r="E14" s="267" t="e">
+      <c r="E14" s="265" t="e">
         <f>E15-E13</f>
         <v>#N/A</v>
       </c>
-      <c r="F14" s="267" t="e">
+      <c r="F14" s="265" t="e">
         <f t="shared" ref="F14:G14" si="3">F15-F13</f>
         <v>#N/A</v>
       </c>
-      <c r="G14" s="267" t="e">
+      <c r="G14" s="265" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
@@ -8790,15 +8776,15 @@
       </c>
       <c r="C15"/>
       <c r="D15" s="130"/>
-      <c r="E15" s="267" t="e">
+      <c r="E15" s="265" t="e">
         <f>IF($D$8=$E$8,IF(NOT(E42=0),E42,E58),E58)</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="267" t="e">
+      <c r="F15" s="265" t="e">
         <f>IF($D$8=$E$8,IF(NOT(F42=0),F42,F58),F58)</f>
         <v>#N/A</v>
       </c>
-      <c r="G15" s="267" t="e">
+      <c r="G15" s="265" t="e">
         <f>IF($D$8=$E$8,IF(NOT(G42=0),G42,G58),G58)</f>
         <v>#N/A</v>
       </c>
@@ -8810,15 +8796,15 @@
       </c>
       <c r="C16"/>
       <c r="D16" s="130"/>
-      <c r="E16" s="267" t="e">
+      <c r="E16" s="265" t="e">
         <f>E17-E15</f>
         <v>#N/A</v>
       </c>
-      <c r="F16" s="267" t="e">
+      <c r="F16" s="265" t="e">
         <f t="shared" ref="F16:G16" si="4">F17-F15</f>
         <v>#N/A</v>
       </c>
-      <c r="G16" s="267" t="e">
+      <c r="G16" s="265" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
@@ -8830,15 +8816,15 @@
       </c>
       <c r="C17"/>
       <c r="D17" s="130"/>
-      <c r="E17" s="267" t="e">
+      <c r="E17" s="265" t="e">
         <f t="shared" ref="E17:G21" si="5">IF($D$8=$E$8,IF(NOT(E44=0),E44,E60),E60)</f>
         <v>#N/A</v>
       </c>
-      <c r="F17" s="267" t="e">
+      <c r="F17" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G17" s="267" t="e">
+      <c r="G17" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8850,15 +8836,15 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="162"/>
-      <c r="E18" s="267" t="e">
+      <c r="E18" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="267" t="e">
+      <c r="F18" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G18" s="267" t="e">
+      <c r="G18" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8870,15 +8856,15 @@
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="130"/>
-      <c r="E19" s="267" t="e">
+      <c r="E19" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="267" t="e">
+      <c r="F19" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G19" s="267" t="e">
+      <c r="G19" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8890,15 +8876,15 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="162"/>
-      <c r="E20" s="267" t="e">
+      <c r="E20" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F20" s="267" t="e">
+      <c r="F20" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G20" s="267" t="e">
+      <c r="G20" s="265" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8910,15 +8896,15 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="166"/>
-      <c r="E21" s="268" t="e">
+      <c r="E21" s="266" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F21" s="268" t="e">
+      <c r="F21" s="266" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G21" s="268" t="e">
+      <c r="G21" s="266" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8926,32 +8912,32 @@
     <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="E22" s="269"/>
-      <c r="F22" s="269"/>
-      <c r="G22" s="269"/>
+      <c r="E22" s="267"/>
+      <c r="F22" s="267"/>
+      <c r="G22" s="267"/>
     </row>
     <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="E23" s="269"/>
-      <c r="F23" s="269"/>
-      <c r="G23" s="269"/>
+      <c r="E23" s="267"/>
+      <c r="F23" s="267"/>
+      <c r="G23" s="267"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B24" s="242" t="s">
+      <c r="B24" s="240" t="s">
         <v>289</v>
       </c>
-      <c r="C24" s="243"/>
-      <c r="D24" s="243"/>
-      <c r="E24" s="270"/>
-      <c r="F24" s="270"/>
-      <c r="G24" s="270"/>
-      <c r="H24" s="243"/>
+      <c r="C24" s="241"/>
+      <c r="D24" s="241"/>
+      <c r="E24" s="268"/>
+      <c r="F24" s="268"/>
+      <c r="G24" s="268"/>
+      <c r="H24" s="241"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="E25" s="271"/>
-      <c r="F25" s="271"/>
-      <c r="G25" s="271"/>
+      <c r="E25" s="269"/>
+      <c r="F25" s="269"/>
+      <c r="G25" s="269"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B26" s="116" t="s">
@@ -8959,135 +8945,135 @@
       </c>
       <c r="C26" s="50"/>
       <c r="D26" s="72"/>
-      <c r="E26" s="272"/>
-      <c r="F26" s="271"/>
-      <c r="G26" s="271"/>
+      <c r="E26" s="270"/>
+      <c r="F26" s="269"/>
+      <c r="G26" s="269"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B27" s="72" t="s">
         <v>91</v>
       </c>
       <c r="C27" s="50"/>
-      <c r="D27" s="228">
+      <c r="D27" s="227">
         <f>Assumptions!D9</f>
         <v>0</v>
       </c>
-      <c r="E27" s="272"/>
-      <c r="F27" s="271"/>
-      <c r="G27" s="271"/>
+      <c r="E27" s="270"/>
+      <c r="F27" s="269"/>
+      <c r="G27" s="269"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B28" s="72" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="50"/>
-      <c r="D28" s="228"/>
+      <c r="D28" s="227"/>
       <c r="E28" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="271"/>
-      <c r="G28" s="271"/>
+      <c r="F28" s="269"/>
+      <c r="G28" s="269"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B29" s="72" t="s">
         <v>190</v>
       </c>
       <c r="C29" s="50"/>
-      <c r="D29" s="230">
+      <c r="D29" s="229">
         <f>Assumptions!D21</f>
         <v>0</v>
       </c>
       <c r="E29" s="112"/>
-      <c r="F29" s="271"/>
-      <c r="G29" s="271"/>
+      <c r="F29" s="269"/>
+      <c r="G29" s="269"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B30" s="72" t="s">
         <v>196</v>
       </c>
       <c r="C30" s="50"/>
-      <c r="D30" s="230">
+      <c r="D30" s="229">
         <f>Assumptions!D22</f>
         <v>0</v>
       </c>
       <c r="E30" s="163"/>
-      <c r="F30" s="271"/>
-      <c r="G30" s="271"/>
+      <c r="F30" s="269"/>
+      <c r="G30" s="269"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B31" s="72" t="s">
         <v>274</v>
       </c>
       <c r="C31" s="50"/>
-      <c r="D31" s="228">
+      <c r="D31" s="227">
         <f>Assumptions!D15</f>
         <v>0</v>
       </c>
       <c r="E31" s="110"/>
-      <c r="F31" s="271"/>
-      <c r="G31" s="271"/>
+      <c r="F31" s="269"/>
+      <c r="G31" s="269"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B32" s="72" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="50"/>
-      <c r="D32" s="228">
+      <c r="D32" s="227">
         <f>Assumptions!D16</f>
         <v>0</v>
       </c>
       <c r="E32" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="271"/>
-      <c r="G32" s="271"/>
+      <c r="F32" s="269"/>
+      <c r="G32" s="269"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="D33" s="232"/>
+      <c r="D33" s="231"/>
       <c r="E33" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="271"/>
-      <c r="G33" s="271"/>
+      <c r="F33" s="269"/>
+      <c r="G33" s="269"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B34" s="72" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="50"/>
-      <c r="D34" s="228">
+      <c r="D34" s="227">
         <f>Assumptions!D11</f>
         <v>0</v>
       </c>
-      <c r="E34" s="273"/>
-      <c r="F34" s="271"/>
-      <c r="G34" s="271"/>
+      <c r="E34" s="271"/>
+      <c r="F34" s="269"/>
+      <c r="G34" s="269"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B35" s="72" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="50"/>
-      <c r="D35" s="228">
+      <c r="D35" s="227">
         <f>Assumptions!D17</f>
         <v>0</v>
       </c>
-      <c r="E35" s="272"/>
-      <c r="F35" s="271"/>
-      <c r="G35" s="271"/>
+      <c r="E35" s="270"/>
+      <c r="F35" s="269"/>
+      <c r="G35" s="269"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="E36" s="274"/>
-      <c r="F36" s="271"/>
-      <c r="G36" s="271"/>
+      <c r="E36" s="272"/>
+      <c r="F36" s="269"/>
+      <c r="G36" s="269"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B37" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="E37" s="271"/>
-      <c r="F37" s="271"/>
-      <c r="G37" s="271"/>
+      <c r="E37" s="269"/>
+      <c r="F37" s="269"/>
+      <c r="G37" s="269"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B38" s="117" t="s">
@@ -9132,15 +9118,15 @@
       <c r="D40" s="130" t="s">
         <v>189</v>
       </c>
-      <c r="E40" s="266" t="str">
+      <c r="E40" s="264" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D40, E$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="F40" s="266" t="str">
+      <c r="F40" s="264" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D40, F$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="G40" s="266" t="str">
+      <c r="G40" s="264" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D40, G$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
@@ -9150,15 +9136,15 @@
         <v>83</v>
       </c>
       <c r="D41" s="130"/>
-      <c r="E41" s="267" t="e">
+      <c r="E41" s="265" t="e">
         <f>E42-E40</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F41" s="267" t="e">
+      <c r="F41" s="265" t="e">
         <f t="shared" ref="F41:G41" si="9">F42-F40</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G41" s="267" t="e">
+      <c r="G41" s="265" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
@@ -9170,15 +9156,15 @@
       <c r="D42" s="130" t="s">
         <v>288</v>
       </c>
-      <c r="E42" s="267" t="e">
+      <c r="E42" s="265" t="e">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D42, E$39, $D$29, , $D$32, $D$34, $D$35)*E40/100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F42" s="267" t="e">
+      <c r="F42" s="265" t="e">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D42, F$39, $D$29, , $D$32, $D$34, $D$35)*F40/100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G42" s="267" t="e">
+      <c r="G42" s="265" t="e">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D42, G$39, $D$29, , $D$32, $D$34, $D$35)*G40/100</f>
         <v>#VALUE!</v>
       </c>
@@ -9188,15 +9174,15 @@
         <v>222</v>
       </c>
       <c r="D43" s="130"/>
-      <c r="E43" s="267" t="e">
+      <c r="E43" s="265" t="e">
         <f>E46-E42</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F43" s="267" t="e">
+      <c r="F43" s="265" t="e">
         <f t="shared" ref="F43:G43" si="10">F46-F42</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G43" s="267" t="e">
+      <c r="G43" s="265" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
@@ -9208,15 +9194,15 @@
       <c r="D44" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="E44" s="267" t="str">
+      <c r="E44" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D44, E$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="F44" s="267" t="str">
+      <c r="F44" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D44, F$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="G44" s="267" t="str">
+      <c r="G44" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D44, G$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
@@ -9229,15 +9215,15 @@
       <c r="D45" s="162" t="s">
         <v>193</v>
       </c>
-      <c r="E45" s="267" t="e">
+      <c r="E45" s="265" t="e">
         <f>-_xll.ciqfunctions.udf.CIQ($D$27, $D45, E$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F45" s="267" t="e">
+      <c r="F45" s="265" t="e">
         <f>-_xll.ciqfunctions.udf.CIQ($D$27, $D45, F$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G45" s="267" t="e">
+      <c r="G45" s="265" t="e">
         <f>-_xll.ciqfunctions.udf.CIQ($D$27, $D45, G$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>#VALUE!</v>
       </c>
@@ -9250,15 +9236,15 @@
       <c r="D46" s="130" t="s">
         <v>192</v>
       </c>
-      <c r="E46" s="267" t="str">
+      <c r="E46" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D46, E$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="F46" s="267" t="str">
+      <c r="F46" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D46, F$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="G46" s="267" t="str">
+      <c r="G46" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D46, G$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
@@ -9271,15 +9257,15 @@
       <c r="D47" s="162" t="s">
         <v>194</v>
       </c>
-      <c r="E47" s="267" t="str">
+      <c r="E47" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D47, E$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="F47" s="267" t="str">
+      <c r="F47" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D47, F$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
-      <c r="G47" s="267" t="str">
+      <c r="G47" s="265" t="str">
         <f>_xll.ciqfunctions.udf.CIQ($D$27, $D47, G$39, $D$29, , $D$32, $D$34, $D$35)</f>
         <v>(Invalid Filing Mode)</v>
       </c>
@@ -9290,55 +9276,55 @@
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="166"/>
-      <c r="E48" s="268" t="e">
+      <c r="E48" s="266" t="e">
         <f>E40/D56*D48</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F48" s="268" t="e">
+      <c r="F48" s="266" t="e">
         <f>F40/E40*E48</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G48" s="268" t="e">
+      <c r="G48" s="266" t="e">
         <f>G40/F40*F48</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B49" s="3"/>
-      <c r="E49" s="271"/>
-      <c r="F49" s="271"/>
-      <c r="G49" s="271"/>
+      <c r="E49" s="269"/>
+      <c r="F49" s="269"/>
+      <c r="G49" s="269"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B50" s="3"/>
-      <c r="E50" s="271"/>
-      <c r="F50" s="271"/>
-      <c r="G50" s="271"/>
+      <c r="E50" s="269"/>
+      <c r="F50" s="269"/>
+      <c r="G50" s="269"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B51" s="242" t="s">
+      <c r="B51" s="240" t="s">
         <v>221</v>
       </c>
-      <c r="C51" s="243"/>
-      <c r="D51" s="243"/>
-      <c r="E51" s="270"/>
-      <c r="F51" s="270"/>
-      <c r="G51" s="270"/>
-      <c r="H51" s="243"/>
+      <c r="C51" s="241"/>
+      <c r="D51" s="241"/>
+      <c r="E51" s="268"/>
+      <c r="F51" s="268"/>
+      <c r="G51" s="268"/>
+      <c r="H51" s="241"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B52" s="3"/>
-      <c r="E52" s="271"/>
-      <c r="F52" s="271"/>
-      <c r="G52" s="271"/>
+      <c r="E52" s="269"/>
+      <c r="F52" s="269"/>
+      <c r="G52" s="269"/>
     </row>
     <row r="53" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B53" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="E53" s="271"/>
-      <c r="F53" s="271"/>
-      <c r="G53" s="271"/>
+      <c r="E53" s="269"/>
+      <c r="F53" s="269"/>
+      <c r="G53" s="269"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B54" s="117" t="s">
@@ -9390,19 +9376,19 @@
         <f>INDEX(IS!21:21,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E56" s="278" t="e">
+      <c r="E56" s="276" t="e">
         <f>D56*(1+E69)</f>
         <v>#N/A</v>
       </c>
-      <c r="F56" s="279" t="e">
+      <c r="F56" s="277" t="e">
         <f>E56*(1+F69)</f>
         <v>#N/A</v>
       </c>
-      <c r="G56" s="279" t="e">
+      <c r="G56" s="277" t="e">
         <f>F56*(1+G69)</f>
         <v>#N/A</v>
       </c>
-      <c r="H56" s="232"/>
+      <c r="H56" s="231"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B57" s="7" t="s">
@@ -9412,19 +9398,19 @@
         <f>INDEX(IS!22:22,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E57" s="280" t="e">
+      <c r="E57" s="278" t="e">
         <f>-E56*E70</f>
         <v>#N/A</v>
       </c>
-      <c r="F57" s="281" t="e">
+      <c r="F57" s="279" t="e">
         <f>-F56*F70</f>
         <v>#N/A</v>
       </c>
-      <c r="G57" s="281" t="e">
+      <c r="G57" s="279" t="e">
         <f>-G56*G70</f>
         <v>#N/A</v>
       </c>
-      <c r="H57" s="232"/>
+      <c r="H57" s="231"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B58" s="7" t="s">
@@ -9434,19 +9420,19 @@
         <f>INDEX(IS!23:23,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E58" s="280" t="e">
+      <c r="E58" s="278" t="e">
         <f t="shared" ref="E58:G58" si="14">E56+E57</f>
         <v>#N/A</v>
       </c>
-      <c r="F58" s="281" t="e">
+      <c r="F58" s="279" t="e">
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-      <c r="G58" s="281" t="e">
+      <c r="G58" s="279" t="e">
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-      <c r="H58" s="232"/>
+      <c r="H58" s="231"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B59" s="7" t="s">
@@ -9456,19 +9442,19 @@
         <f>INDEX(IS!27:27,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E59" s="280" t="e">
+      <c r="E59" s="278" t="e">
         <f>-E56*E71+E72</f>
         <v>#N/A</v>
       </c>
-      <c r="F59" s="281" t="e">
+      <c r="F59" s="279" t="e">
         <f t="shared" ref="F59:G59" si="15">-F56*F71+F72</f>
         <v>#N/A</v>
       </c>
-      <c r="G59" s="281" t="e">
+      <c r="G59" s="279" t="e">
         <f t="shared" si="15"/>
         <v>#N/A</v>
       </c>
-      <c r="H59" s="232"/>
+      <c r="H59" s="231"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B60" s="7" t="s">
@@ -9478,19 +9464,19 @@
         <f>INDEX(IS!28:28,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E60" s="280" t="e">
+      <c r="E60" s="278" t="e">
         <f t="shared" ref="E60:G60" si="16">E58+E59</f>
         <v>#N/A</v>
       </c>
-      <c r="F60" s="281" t="e">
+      <c r="F60" s="279" t="e">
         <f t="shared" si="16"/>
         <v>#N/A</v>
       </c>
-      <c r="G60" s="281" t="e">
+      <c r="G60" s="279" t="e">
         <f t="shared" si="16"/>
         <v>#N/A</v>
       </c>
-      <c r="H60" s="232"/>
+      <c r="H60" s="231"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B61" s="34" t="s">
@@ -9501,19 +9487,19 @@
         <f>INDEX(IS!29:29,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E61" s="280" t="e">
+      <c r="E61" s="278" t="e">
         <f>-E56*E73</f>
         <v>#N/A</v>
       </c>
-      <c r="F61" s="281" t="e">
+      <c r="F61" s="279" t="e">
         <f>-F56*F73</f>
         <v>#N/A</v>
       </c>
-      <c r="G61" s="281" t="e">
+      <c r="G61" s="279" t="e">
         <f>-G56*G73</f>
         <v>#N/A</v>
       </c>
-      <c r="H61" s="232"/>
+      <c r="H61" s="231"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B62" s="12" t="s">
@@ -9524,19 +9510,19 @@
         <f>INDEX(IS!30:30,MATCH(D$54,IS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E62" s="280" t="e">
+      <c r="E62" s="278" t="e">
         <f>E60+E61</f>
         <v>#N/A</v>
       </c>
-      <c r="F62" s="281" t="e">
+      <c r="F62" s="279" t="e">
         <f t="shared" ref="F62:G62" si="17">F60+F61</f>
         <v>#N/A</v>
       </c>
-      <c r="G62" s="281" t="e">
+      <c r="G62" s="279" t="e">
         <f t="shared" si="17"/>
         <v>#N/A</v>
       </c>
-      <c r="H62" s="232"/>
+      <c r="H62" s="231"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B63" s="34" t="s">
@@ -9547,19 +9533,19 @@
         <f>INDEX(CFS!25:25,MATCH(D$54,CFS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E63" s="280" t="e">
+      <c r="E63" s="278" t="e">
         <f>-E56*E74</f>
         <v>#N/A</v>
       </c>
-      <c r="F63" s="281" t="e">
+      <c r="F63" s="279" t="e">
         <f>-F56*F74</f>
         <v>#N/A</v>
       </c>
-      <c r="G63" s="281" t="e">
+      <c r="G63" s="279" t="e">
         <f>-G56*G74</f>
         <v>#N/A</v>
       </c>
-      <c r="H63" s="232"/>
+      <c r="H63" s="231"/>
     </row>
     <row r="64" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B64" s="4" t="s">
@@ -9570,34 +9556,34 @@
         <f>INDEX(BS!29:29,MATCH(D$54,BS!$19:$19,0))-INDEX(BS!46:46,MATCH(D$54,BS!$19:$19,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E64" s="282" t="e">
+      <c r="E64" s="280" t="e">
         <f>E56*E75</f>
         <v>#N/A</v>
       </c>
-      <c r="F64" s="283" t="e">
+      <c r="F64" s="281" t="e">
         <f>F56*F75</f>
         <v>#N/A</v>
       </c>
-      <c r="G64" s="283" t="e">
+      <c r="G64" s="281" t="e">
         <f>G56*G75</f>
         <v>#N/A</v>
       </c>
-      <c r="H64" s="232"/>
+      <c r="H64" s="231"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="E65" s="284"/>
-      <c r="F65" s="284"/>
-      <c r="G65" s="284"/>
-      <c r="H65" s="232"/>
+      <c r="E65" s="282"/>
+      <c r="F65" s="282"/>
+      <c r="G65" s="282"/>
+      <c r="H65" s="231"/>
     </row>
     <row r="66" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B66" s="116" t="s">
         <v>283</v>
       </c>
-      <c r="E66" s="284"/>
-      <c r="F66" s="284"/>
-      <c r="G66" s="284"/>
-      <c r="H66" s="232"/>
+      <c r="E66" s="282"/>
+      <c r="F66" s="282"/>
+      <c r="G66" s="282"/>
+      <c r="H66" s="231"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B67" s="117" t="s">
@@ -9608,19 +9594,19 @@
         <f>$E$54+COLUMN(D54)-COLUMN($E$54)</f>
         <v>1899</v>
       </c>
-      <c r="E67" s="285">
+      <c r="E67" s="283">
         <f>YEAR($D$30)</f>
         <v>1900</v>
       </c>
-      <c r="F67" s="285">
+      <c r="F67" s="283">
         <f>$E$54+COLUMN(F67)-COLUMN($E$54)</f>
         <v>1901</v>
       </c>
-      <c r="G67" s="285">
+      <c r="G67" s="283">
         <f t="shared" ref="G67" si="18">$E$54+COLUMN(G67)-COLUMN($E$54)</f>
         <v>1902</v>
       </c>
-      <c r="H67" s="232"/>
+      <c r="H67" s="231"/>
     </row>
     <row r="68" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B68" s="121"/>
@@ -9629,131 +9615,131 @@
         <f>"FY"&amp;D67</f>
         <v>FY1899</v>
       </c>
-      <c r="E68" s="286" t="str">
+      <c r="E68" s="284" t="str">
         <f>"FY"&amp;E67</f>
         <v>FY1900</v>
       </c>
-      <c r="F68" s="286" t="str">
+      <c r="F68" s="284" t="str">
         <f t="shared" ref="F68:G68" si="19">"FY"&amp;F67</f>
         <v>FY1901</v>
       </c>
-      <c r="G68" s="286" t="str">
+      <c r="G68" s="284" t="str">
         <f t="shared" si="19"/>
         <v>FY1902</v>
       </c>
-      <c r="H68" s="232"/>
+      <c r="H68" s="231"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B69" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D69" s="275" t="e" cm="1">
+      <c r="D69" s="273" t="e" cm="1">
         <f t="array" ref="D69">INDEX(IS!21:21,MATCH(D$54,IS!$19:$19,0))/INDEX(IS!21:21,MATCH(D$54,IS!$19:$19,0)-1)-1</f>
         <v>#N/A</v>
       </c>
-      <c r="E69" s="287"/>
-      <c r="F69" s="288"/>
-      <c r="G69" s="288"/>
-      <c r="H69" s="232"/>
+      <c r="E69" s="285"/>
+      <c r="F69" s="286"/>
+      <c r="G69" s="286"/>
+      <c r="H69" s="231"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B70" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="D70" s="276" t="e">
+      <c r="D70" s="274" t="e">
         <f>-D57/D56</f>
         <v>#N/A</v>
       </c>
-      <c r="E70" s="289"/>
-      <c r="F70" s="290"/>
-      <c r="G70" s="290"/>
-      <c r="H70" s="232"/>
+      <c r="E70" s="287"/>
+      <c r="F70" s="288"/>
+      <c r="G70" s="288"/>
+      <c r="H70" s="231"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B71" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="D71" s="276"/>
-      <c r="E71" s="289"/>
-      <c r="F71" s="290"/>
-      <c r="G71" s="290"/>
-      <c r="H71" s="232"/>
+      <c r="D71" s="274"/>
+      <c r="E71" s="287"/>
+      <c r="F71" s="288"/>
+      <c r="G71" s="288"/>
+      <c r="H71" s="231"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B72" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="D72" s="276"/>
-      <c r="E72" s="280"/>
-      <c r="F72" s="281"/>
-      <c r="G72" s="281"/>
-      <c r="H72" s="232"/>
+      <c r="D72" s="274"/>
+      <c r="E72" s="289"/>
+      <c r="F72" s="290"/>
+      <c r="G72" s="290"/>
+      <c r="H72" s="231"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B73" s="34" t="s">
         <v>290</v>
       </c>
       <c r="C73" s="2"/>
-      <c r="D73" s="276" t="e">
+      <c r="D73" s="274" t="e">
         <f>-D61/D56</f>
         <v>#N/A</v>
       </c>
       <c r="E73" s="291"/>
       <c r="F73" s="292"/>
       <c r="G73" s="292"/>
-      <c r="H73" s="232"/>
+      <c r="H73" s="231"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B74" s="34" t="s">
         <v>291</v>
       </c>
       <c r="C74" s="2"/>
-      <c r="D74" s="276" t="e">
+      <c r="D74" s="274" t="e">
         <f>-D63/D56</f>
         <v>#N/A</v>
       </c>
       <c r="E74" s="291"/>
       <c r="F74" s="292"/>
       <c r="G74" s="292"/>
-      <c r="H74" s="232"/>
+      <c r="H74" s="231"/>
     </row>
     <row r="75" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B75" s="4" t="s">
         <v>292</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="277" t="e">
+      <c r="D75" s="275" t="e">
         <f>D64/D56</f>
         <v>#N/A</v>
       </c>
       <c r="E75" s="293"/>
       <c r="F75" s="294"/>
       <c r="G75" s="294"/>
-      <c r="H75" s="232"/>
+      <c r="H75" s="231"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="E76" s="232"/>
-      <c r="F76" s="232"/>
-      <c r="G76" s="232"/>
-      <c r="H76" s="232"/>
+      <c r="E76" s="231"/>
+      <c r="F76" s="231"/>
+      <c r="G76" s="231"/>
+      <c r="H76" s="231"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="E77" s="232"/>
-      <c r="F77" s="232"/>
-      <c r="G77" s="232"/>
-      <c r="H77" s="232"/>
+      <c r="E77" s="231"/>
+      <c r="F77" s="231"/>
+      <c r="G77" s="231"/>
+      <c r="H77" s="231"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="E78" s="232"/>
-      <c r="F78" s="232"/>
-      <c r="G78" s="232"/>
-      <c r="H78" s="232"/>
+      <c r="E78" s="231"/>
+      <c r="F78" s="231"/>
+      <c r="G78" s="231"/>
+      <c r="H78" s="231"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="E79" s="232"/>
-      <c r="F79" s="232"/>
-      <c r="G79" s="232"/>
-      <c r="H79" s="232"/>
+      <c r="E79" s="231"/>
+      <c r="F79" s="231"/>
+      <c r="G79" s="231"/>
+      <c r="H79" s="231"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>